<commit_message>
Add latest ONS estimates
</commit_message>
<xml_diff>
--- a/data/ons-deaths/explore/evaluation_of_ons_estimates.xlsx
+++ b/data/ons-deaths/explore/evaluation_of_ons_estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\covid-stats\data\ons-deaths\explore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5AB337-A233-4366-AD61-EB63728CF688}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EDF98B-F2E2-41EC-A5FA-DCB4F8D88D61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="0" windowWidth="21600" windowHeight="15540" activeTab="2" xr2:uid="{A515F7DA-6FDB-438E-B4AB-3C334154F930}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{A515F7DA-6FDB-438E-B4AB-3C334154F930}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Week number</t>
   </si>
   <si>
     <t>Week ended</t>
+  </si>
+  <si>
+    <t>week ended</t>
+  </si>
+  <si>
+    <t>estimate</t>
   </si>
 </sst>
 </file>
@@ -43,7 +49,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="General_)"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,14 +143,8 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,6 +165,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -599,7 +605,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -613,60 +619,29 @@
     <xf numFmtId="15" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="379" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="0" xfId="379" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="379" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="4" fillId="4" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1100,7 +1075,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Overlay of ONS estimates for deaths per week</a:t>
+              <a:t>Overlay of ONS estimates for deaths occurring each week</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1168,10 +1143,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AS$2:$BD$2</c:f>
+              <c:f>data!$AS$2:$ZZ$2</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="658"/>
                 <c:pt idx="0">
                   <c:v>44127</c:v>
                 </c:pt>
@@ -1207,6 +1182,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1258,10 +1236,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AS$2:$BD$2</c:f>
+              <c:f>data!$AS$2:$ZZ$2</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="658"/>
                 <c:pt idx="0">
                   <c:v>44127</c:v>
                 </c:pt>
@@ -1297,6 +1275,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1353,10 +1334,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AS$2:$BD$2</c:f>
+              <c:f>data!$AS$2:$ZZ$2</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="658"/>
                 <c:pt idx="0">
                   <c:v>44127</c:v>
                 </c:pt>
@@ -1392,6 +1373,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1449,10 +1433,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AS$2:$BD$2</c:f>
+              <c:f>data!$AS$2:$ZZ$2</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="658"/>
                 <c:pt idx="0">
                   <c:v>44127</c:v>
                 </c:pt>
@@ -1488,6 +1472,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1548,10 +1535,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AS$2:$BD$2</c:f>
+              <c:f>data!$AS$2:$ZZ$2</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="658"/>
                 <c:pt idx="0">
                   <c:v>44127</c:v>
                 </c:pt>
@@ -1587,6 +1574,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1650,10 +1640,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AS$2:$BD$2</c:f>
+              <c:f>data!$AS$2:$ZZ$2</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="658"/>
                 <c:pt idx="0">
                   <c:v>44127</c:v>
                 </c:pt>
@@ -1689,6 +1679,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1755,10 +1748,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AS$2:$BD$2</c:f>
+              <c:f>data!$AS$2:$ZZ$2</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="658"/>
                 <c:pt idx="0">
                   <c:v>44127</c:v>
                 </c:pt>
@@ -1794,6 +1787,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1865,10 +1861,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AS$2:$BD$2</c:f>
+              <c:f>data!$AS$2:$ZZ$2</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="658"/>
                 <c:pt idx="0">
                   <c:v>44127</c:v>
                 </c:pt>
@@ -1904,6 +1900,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1978,10 +1977,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AS$2:$BD$2</c:f>
+              <c:f>data!$AS$2:$ZZ$2</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="658"/>
                 <c:pt idx="0">
                   <c:v>44127</c:v>
                 </c:pt>
@@ -2017,6 +2016,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2094,10 +2096,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AS$2:$BD$2</c:f>
+              <c:f>data!$AS$2:$ZZ$2</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="658"/>
                 <c:pt idx="0">
                   <c:v>44127</c:v>
                 </c:pt>
@@ -2133,6 +2135,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2213,10 +2218,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AS$2:$BD$2</c:f>
+              <c:f>data!$AS$2:$ZZ$2</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="658"/>
                 <c:pt idx="0">
                   <c:v>44127</c:v>
                 </c:pt>
@@ -2252,6 +2257,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2305,6 +2313,137 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000A-F363-404A-9F48-CECF406857D0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$AS$2:$ZZ$2</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="658"/>
+                <c:pt idx="0">
+                  <c:v>44127</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44134</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44141</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44148</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44155</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44162</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44169</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44176</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44183</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44190</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44211</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AS$15:$ZZ$15</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="658"/>
+                <c:pt idx="0">
+                  <c:v>11062</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11393</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11755</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12348</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12313</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12443</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12656</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13140</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13413</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14747</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16645</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D9F9-4C3B-AA97-5A99ABF51506}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2345,7 +2484,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -3406,13 +3545,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D1BBA0-D981-49C0-9749-BCE3B566D49F}">
-  <dimension ref="A1:BD14"/>
+  <dimension ref="A1:DF15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="AS3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="BC16" sqref="BC16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3430,7 +3569,7 @@
     <col min="56" max="56" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:110" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3597,7 +3736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:56" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:110" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -3764,534 +3903,540 @@
       <c r="BD2" s="6">
         <v>44204</v>
       </c>
+      <c r="BE2" s="6">
+        <v>44211</v>
+      </c>
     </row>
-    <row r="3" spans="1:56" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="18">
+    <row r="3" spans="1:110" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
         <v>43</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3">
         <v>12431</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3">
         <v>12139</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3">
         <v>11746</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3">
         <v>10914</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3">
         <v>11094</v>
       </c>
-      <c r="H3" s="20">
+      <c r="H3">
         <v>10710</v>
       </c>
-      <c r="I3" s="20">
+      <c r="I3">
         <v>10877</v>
       </c>
-      <c r="J3" s="20">
+      <c r="J3">
         <v>10795</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3">
         <v>10647</v>
       </c>
-      <c r="L3" s="20">
+      <c r="L3">
         <v>10984</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3">
         <v>10834</v>
       </c>
-      <c r="N3" s="20">
+      <c r="N3">
         <v>11401</v>
       </c>
-      <c r="O3" s="20">
+      <c r="O3">
         <v>13787</v>
       </c>
-      <c r="P3" s="20">
+      <c r="P3">
         <v>17897</v>
       </c>
-      <c r="Q3" s="20">
+      <c r="Q3">
         <v>22038</v>
       </c>
-      <c r="R3" s="20">
+      <c r="R3">
         <v>20922</v>
       </c>
-      <c r="S3" s="20">
+      <c r="S3">
         <v>18694</v>
       </c>
-      <c r="T3" s="20">
+      <c r="T3">
         <v>15827</v>
       </c>
-      <c r="U3" s="20">
+      <c r="U3">
         <v>13728</v>
       </c>
-      <c r="V3" s="20">
+      <c r="V3">
         <v>11970</v>
       </c>
-      <c r="W3" s="20">
+      <c r="W3">
         <v>11360</v>
       </c>
-      <c r="X3" s="20">
+      <c r="X3">
         <v>10222</v>
       </c>
-      <c r="Y3" s="20">
+      <c r="Y3">
         <v>9985</v>
       </c>
-      <c r="Z3" s="20">
+      <c r="Z3">
         <v>9468</v>
       </c>
-      <c r="AA3" s="20">
+      <c r="AA3">
         <v>9227</v>
       </c>
-      <c r="AB3" s="20">
+      <c r="AB3">
         <v>9670</v>
       </c>
-      <c r="AC3" s="20">
+      <c r="AC3">
         <v>8754</v>
       </c>
-      <c r="AD3" s="20">
+      <c r="AD3">
         <v>8682</v>
       </c>
-      <c r="AE3" s="20">
+      <c r="AE3" s="14">
         <v>8893</v>
       </c>
-      <c r="AF3" s="20">
+      <c r="AF3" s="14">
         <v>9082</v>
       </c>
-      <c r="AG3" s="20">
+      <c r="AG3" s="14">
         <v>8854</v>
       </c>
-      <c r="AH3" s="20">
+      <c r="AH3" s="14">
         <v>9013</v>
       </c>
-      <c r="AI3" s="20">
+      <c r="AI3" s="14">
         <v>10148</v>
       </c>
-      <c r="AJ3" s="20">
+      <c r="AJ3" s="14">
         <v>8813</v>
       </c>
-      <c r="AK3" s="20">
+      <c r="AK3" s="14">
         <v>8651</v>
       </c>
-      <c r="AL3" s="20">
+      <c r="AL3" s="14">
         <v>9065</v>
       </c>
-      <c r="AM3" s="20">
+      <c r="AM3" s="14">
         <v>9128</v>
       </c>
-      <c r="AN3" s="20">
+      <c r="AN3" s="14">
         <v>9439</v>
       </c>
-      <c r="AO3" s="20">
+      <c r="AO3" s="14">
         <v>9598</v>
       </c>
-      <c r="AP3" s="20">
+      <c r="AP3" s="14">
         <v>9945</v>
       </c>
-      <c r="AQ3" s="20">
+      <c r="AQ3" s="14">
         <v>10337</v>
       </c>
-      <c r="AR3" s="21">
+      <c r="AR3" s="14">
         <v>10383</v>
       </c>
-      <c r="AS3" s="22">
+      <c r="AS3" s="14">
         <v>10809</v>
       </c>
-      <c r="AT3" s="20"/>
-      <c r="AU3" s="20"/>
-      <c r="AV3" s="20"/>
-      <c r="AW3" s="20"/>
-      <c r="AX3" s="20"/>
-      <c r="AY3" s="20"/>
-      <c r="AZ3" s="20"/>
-      <c r="BA3" s="20"/>
-      <c r="BB3" s="20"/>
-      <c r="BC3" s="20"/>
-      <c r="BD3" s="20"/>
+      <c r="AT3" s="14"/>
+      <c r="AU3" s="14"/>
+      <c r="AV3" s="14"/>
+      <c r="AW3" s="14"/>
+      <c r="AX3" s="14"/>
+      <c r="AY3" s="14"/>
+      <c r="AZ3" s="14"/>
+      <c r="BA3" s="14"/>
+      <c r="BB3" s="14"/>
+      <c r="BC3" s="14"/>
+      <c r="BD3" s="14"/>
+      <c r="BE3" s="7"/>
     </row>
-    <row r="4" spans="1:56" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="18">
+    <row r="4" spans="1:110" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>44</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4">
         <v>12431</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4">
         <v>12139</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4">
         <v>11746</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4">
         <v>10914</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4">
         <v>11094</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4">
         <v>10710</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4">
         <v>10877</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4">
         <v>10795</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4">
         <v>10647</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4">
         <v>10984</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4">
         <v>10834</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4">
         <v>11401</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4">
         <v>13787</v>
       </c>
-      <c r="P4" s="10">
+      <c r="P4">
         <v>17897</v>
       </c>
-      <c r="Q4" s="10">
+      <c r="Q4">
         <v>22038</v>
       </c>
-      <c r="R4" s="10">
+      <c r="R4">
         <v>20922</v>
       </c>
-      <c r="S4" s="10">
+      <c r="S4">
         <v>18694</v>
       </c>
-      <c r="T4" s="10">
+      <c r="T4">
         <v>15827</v>
       </c>
-      <c r="U4" s="10">
+      <c r="U4">
         <v>13728</v>
       </c>
-      <c r="V4" s="10">
+      <c r="V4">
         <v>11970</v>
       </c>
-      <c r="W4" s="10">
+      <c r="W4">
         <v>11360</v>
       </c>
-      <c r="X4" s="10">
+      <c r="X4">
         <v>10222</v>
       </c>
-      <c r="Y4" s="10">
+      <c r="Y4">
         <v>9985</v>
       </c>
-      <c r="Z4" s="10">
+      <c r="Z4">
         <v>9468</v>
       </c>
-      <c r="AA4" s="10">
+      <c r="AA4">
         <v>9227</v>
       </c>
-      <c r="AB4" s="10">
+      <c r="AB4">
         <v>9670</v>
       </c>
-      <c r="AC4" s="10">
+      <c r="AC4">
         <v>8754</v>
       </c>
-      <c r="AD4" s="10">
+      <c r="AD4">
         <v>8682</v>
       </c>
-      <c r="AE4" s="10">
+      <c r="AE4" s="14">
         <v>8893</v>
       </c>
-      <c r="AF4" s="10">
+      <c r="AF4" s="14">
         <v>9082</v>
       </c>
-      <c r="AG4" s="10">
+      <c r="AG4" s="14">
         <v>8854</v>
       </c>
-      <c r="AH4" s="10">
+      <c r="AH4" s="14">
         <v>9013</v>
       </c>
-      <c r="AI4" s="10">
+      <c r="AI4" s="14">
         <v>10148</v>
       </c>
-      <c r="AJ4" s="10">
+      <c r="AJ4" s="14">
         <v>8813</v>
       </c>
-      <c r="AK4" s="10">
+      <c r="AK4" s="14">
         <v>8651</v>
       </c>
-      <c r="AL4" s="10">
+      <c r="AL4" s="14">
         <v>9065</v>
       </c>
-      <c r="AM4" s="10">
+      <c r="AM4" s="14">
         <v>9128</v>
       </c>
-      <c r="AN4" s="10">
+      <c r="AN4" s="14">
         <v>9439</v>
       </c>
-      <c r="AO4" s="10">
+      <c r="AO4" s="14">
         <v>9598</v>
       </c>
-      <c r="AP4" s="10">
+      <c r="AP4" s="14">
         <v>9945</v>
       </c>
-      <c r="AQ4" s="10">
+      <c r="AQ4" s="14">
         <v>10337</v>
       </c>
-      <c r="AR4" s="11">
+      <c r="AR4" s="14">
         <v>10383</v>
       </c>
-      <c r="AS4" s="11">
+      <c r="AS4" s="14">
         <v>10809</v>
       </c>
-      <c r="AT4" s="17">
+      <c r="AT4" s="14">
         <v>10658</v>
       </c>
-      <c r="AU4" s="10"/>
-      <c r="AV4" s="10"/>
-      <c r="AW4" s="10"/>
-      <c r="AX4" s="10"/>
-      <c r="AY4" s="10"/>
-      <c r="AZ4" s="10"/>
-      <c r="BA4" s="10"/>
-      <c r="BB4" s="10"/>
-      <c r="BC4" s="10"/>
-      <c r="BD4" s="10"/>
+      <c r="AU4" s="14"/>
+      <c r="AV4" s="14"/>
+      <c r="AW4" s="14"/>
+      <c r="AX4" s="14"/>
+      <c r="AY4" s="14"/>
+      <c r="AZ4" s="14"/>
+      <c r="BA4" s="14"/>
+      <c r="BB4" s="14"/>
+      <c r="BC4" s="14"/>
+      <c r="BD4" s="14"/>
+      <c r="BE4" s="7"/>
     </row>
-    <row r="5" spans="1:56" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="18">
+    <row r="5" spans="1:110" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>45</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5">
         <v>12431</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5">
         <v>12139</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5">
         <v>11746</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5">
         <v>10914</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5">
         <v>11094</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5">
         <v>10710</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5">
         <v>10877</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5">
         <v>10795</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5">
         <v>10647</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5">
         <v>10984</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5">
         <v>10834</v>
       </c>
-      <c r="N5" s="10">
+      <c r="N5">
         <v>11401</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5">
         <v>13787</v>
       </c>
-      <c r="P5" s="10">
+      <c r="P5">
         <v>17897</v>
       </c>
-      <c r="Q5" s="10">
+      <c r="Q5">
         <v>22038</v>
       </c>
-      <c r="R5" s="10">
+      <c r="R5">
         <v>20922</v>
       </c>
-      <c r="S5" s="10">
+      <c r="S5">
         <v>18694</v>
       </c>
-      <c r="T5" s="10">
+      <c r="T5">
         <v>15827</v>
       </c>
-      <c r="U5" s="10">
+      <c r="U5">
         <v>13728</v>
       </c>
-      <c r="V5" s="10">
+      <c r="V5">
         <v>11970</v>
       </c>
-      <c r="W5" s="10">
+      <c r="W5">
         <v>11360</v>
       </c>
-      <c r="X5" s="10">
+      <c r="X5">
         <v>10222</v>
       </c>
-      <c r="Y5" s="10">
+      <c r="Y5">
         <v>9985</v>
       </c>
-      <c r="Z5" s="10">
+      <c r="Z5">
         <v>9468</v>
       </c>
-      <c r="AA5" s="10">
+      <c r="AA5">
         <v>9227</v>
       </c>
-      <c r="AB5" s="10">
+      <c r="AB5">
         <v>9676</v>
       </c>
-      <c r="AC5" s="10">
+      <c r="AC5">
         <v>8757</v>
       </c>
-      <c r="AD5" s="10">
+      <c r="AD5">
         <v>8692</v>
       </c>
-      <c r="AE5" s="10">
+      <c r="AE5" s="14">
         <v>8902</v>
       </c>
-      <c r="AF5" s="10">
+      <c r="AF5" s="14">
         <v>9089</v>
       </c>
-      <c r="AG5" s="10">
+      <c r="AG5" s="14">
         <v>8859</v>
       </c>
-      <c r="AH5" s="10">
+      <c r="AH5" s="14">
         <v>9016</v>
       </c>
-      <c r="AI5" s="10">
+      <c r="AI5" s="14">
         <v>10149</v>
       </c>
-      <c r="AJ5" s="10">
+      <c r="AJ5" s="14">
         <v>8827</v>
       </c>
-      <c r="AK5" s="10">
+      <c r="AK5" s="14">
         <v>8662</v>
       </c>
-      <c r="AL5" s="10">
+      <c r="AL5" s="14">
         <v>9057</v>
       </c>
-      <c r="AM5" s="10">
+      <c r="AM5" s="14">
         <v>9138</v>
       </c>
-      <c r="AN5" s="10">
+      <c r="AN5" s="14">
         <v>9449</v>
       </c>
-      <c r="AO5" s="10">
+      <c r="AO5" s="14">
         <v>9596</v>
       </c>
-      <c r="AP5" s="10">
+      <c r="AP5" s="14">
         <v>9955</v>
       </c>
-      <c r="AQ5" s="10">
+      <c r="AQ5" s="14">
         <v>10343</v>
       </c>
-      <c r="AR5" s="11">
+      <c r="AR5" s="14">
         <v>10372</v>
       </c>
-      <c r="AS5" s="11">
+      <c r="AS5" s="14">
         <v>11038</v>
       </c>
-      <c r="AT5" s="11">
+      <c r="AT5" s="14">
         <v>11475</v>
       </c>
-      <c r="AU5" s="10">
+      <c r="AU5" s="14">
         <v>12157</v>
       </c>
-      <c r="AV5" s="10"/>
-      <c r="AW5" s="10"/>
-      <c r="AX5" s="10"/>
-      <c r="AY5" s="10"/>
-      <c r="AZ5" s="10"/>
-      <c r="BA5" s="10"/>
-      <c r="BB5" s="10"/>
-      <c r="BC5" s="10"/>
-      <c r="BD5" s="10"/>
+      <c r="AV5" s="14"/>
+      <c r="AW5" s="14"/>
+      <c r="AX5" s="14"/>
+      <c r="AY5" s="14"/>
+      <c r="AZ5" s="14"/>
+      <c r="BA5" s="14"/>
+      <c r="BB5" s="14"/>
+      <c r="BC5" s="14"/>
+      <c r="BD5" s="14"/>
+      <c r="BE5" s="7"/>
     </row>
-    <row r="6" spans="1:56" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="18">
+    <row r="6" spans="1:110" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>46</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6">
         <v>12431</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6">
         <v>12139</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6">
         <v>11746</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6">
         <v>10914</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6">
         <v>11094</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6">
         <v>10710</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6">
         <v>10877</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6">
         <v>10795</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6">
         <v>10647</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6">
         <v>10984</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6">
         <v>10834</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6">
         <v>11401</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6">
         <v>13787</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P6">
         <v>17897</v>
       </c>
-      <c r="Q6" s="14">
+      <c r="Q6">
         <v>22038</v>
       </c>
-      <c r="R6" s="14">
+      <c r="R6">
         <v>20922</v>
       </c>
-      <c r="S6" s="14">
+      <c r="S6">
         <v>18694</v>
       </c>
-      <c r="T6" s="14">
+      <c r="T6">
         <v>15825</v>
       </c>
-      <c r="U6" s="14">
+      <c r="U6">
         <v>13712</v>
       </c>
-      <c r="V6" s="14">
+      <c r="V6">
         <v>11948</v>
       </c>
-      <c r="W6" s="14">
+      <c r="W6">
         <v>11353</v>
       </c>
-      <c r="X6" s="14">
+      <c r="X6">
         <v>10216</v>
       </c>
-      <c r="Y6" s="14">
+      <c r="Y6">
         <v>9976</v>
       </c>
-      <c r="Z6" s="14">
+      <c r="Z6">
         <v>9469</v>
       </c>
-      <c r="AA6" s="14">
+      <c r="AA6">
         <v>9214</v>
       </c>
-      <c r="AB6" s="14">
+      <c r="AB6">
         <v>9676</v>
       </c>
-      <c r="AC6" s="14">
+      <c r="AC6">
         <v>8755</v>
       </c>
-      <c r="AD6" s="14">
+      <c r="AD6">
         <v>8686</v>
       </c>
       <c r="AE6" s="14">
@@ -4342,1220 +4487,1419 @@
       <c r="AT6" s="14">
         <v>11405</v>
       </c>
-      <c r="AU6" s="16">
+      <c r="AU6" s="14">
         <v>11816</v>
       </c>
-      <c r="AV6" s="15">
+      <c r="AV6" s="14">
         <v>12643</v>
       </c>
-      <c r="AW6" s="20"/>
-      <c r="AX6" s="20"/>
-      <c r="AY6" s="20"/>
-      <c r="AZ6" s="20"/>
-      <c r="BA6" s="20"/>
-      <c r="BB6" s="20"/>
-      <c r="BC6" s="20"/>
-      <c r="BD6" s="20"/>
+      <c r="AW6" s="14"/>
+      <c r="AX6" s="14"/>
+      <c r="AY6" s="14"/>
+      <c r="AZ6" s="14"/>
+      <c r="BA6" s="14"/>
+      <c r="BB6" s="14"/>
+      <c r="BC6" s="14"/>
+      <c r="BD6" s="14"/>
+      <c r="BE6" s="7"/>
     </row>
-    <row r="7" spans="1:56" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="18">
+    <row r="7" spans="1:110" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
         <v>47</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7">
         <v>12431</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7">
         <v>12139</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7">
         <v>11746</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7">
         <v>10914</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7">
         <v>11094</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7">
         <v>10710</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7">
         <v>10877</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7">
         <v>10795</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7">
         <v>10647</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7">
         <v>10984</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7">
         <v>10834</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7">
         <v>11401</v>
       </c>
-      <c r="O7" s="8">
+      <c r="O7">
         <v>13787</v>
       </c>
-      <c r="P7" s="8">
+      <c r="P7">
         <v>17897</v>
       </c>
-      <c r="Q7" s="8">
+      <c r="Q7">
         <v>22038</v>
       </c>
-      <c r="R7" s="8">
+      <c r="R7">
         <v>20922</v>
       </c>
-      <c r="S7" s="8">
+      <c r="S7">
         <v>18694</v>
       </c>
-      <c r="T7" s="8">
+      <c r="T7">
         <v>15825</v>
       </c>
-      <c r="U7" s="8">
+      <c r="U7">
         <v>13712</v>
       </c>
-      <c r="V7" s="8">
+      <c r="V7">
         <v>11948</v>
       </c>
-      <c r="W7" s="8">
+      <c r="W7">
         <v>11354</v>
       </c>
-      <c r="X7" s="8">
+      <c r="X7">
         <v>10220</v>
       </c>
-      <c r="Y7" s="8">
+      <c r="Y7">
         <v>9975</v>
       </c>
-      <c r="Z7" s="8">
+      <c r="Z7">
         <v>9462</v>
       </c>
-      <c r="AA7" s="8">
+      <c r="AA7">
         <v>9220</v>
       </c>
-      <c r="AB7" s="8">
+      <c r="AB7">
         <v>9671</v>
       </c>
-      <c r="AC7" s="8">
+      <c r="AC7">
         <v>8746</v>
       </c>
-      <c r="AD7" s="8">
+      <c r="AD7">
         <v>8682</v>
       </c>
-      <c r="AE7" s="8">
+      <c r="AE7" s="14">
         <v>8907</v>
       </c>
-      <c r="AF7" s="8">
+      <c r="AF7" s="14">
         <v>9090</v>
       </c>
-      <c r="AG7" s="8">
+      <c r="AG7" s="14">
         <v>8874</v>
       </c>
-      <c r="AH7" s="8">
+      <c r="AH7" s="14">
         <v>9009</v>
       </c>
-      <c r="AI7" s="8">
+      <c r="AI7" s="14">
         <v>10153</v>
       </c>
-      <c r="AJ7" s="8">
+      <c r="AJ7" s="14">
         <v>8840</v>
       </c>
-      <c r="AK7" s="8">
+      <c r="AK7" s="14">
         <v>8675</v>
       </c>
-      <c r="AL7" s="8">
+      <c r="AL7" s="14">
         <v>9061</v>
       </c>
-      <c r="AM7" s="8">
+      <c r="AM7" s="14">
         <v>9140</v>
       </c>
-      <c r="AN7" s="8">
+      <c r="AN7" s="14">
         <v>9460</v>
       </c>
-      <c r="AO7" s="8">
+      <c r="AO7" s="14">
         <v>9605</v>
       </c>
-      <c r="AP7" s="8">
+      <c r="AP7" s="14">
         <v>9990</v>
       </c>
-      <c r="AQ7" s="8">
+      <c r="AQ7" s="14">
         <v>10351</v>
       </c>
-      <c r="AR7" s="8">
+      <c r="AR7" s="14">
         <v>10386</v>
       </c>
-      <c r="AS7" s="8">
+      <c r="AS7" s="14">
         <v>11092</v>
       </c>
-      <c r="AT7" s="8">
+      <c r="AT7" s="14">
         <v>11442</v>
       </c>
-      <c r="AU7" s="9">
+      <c r="AU7" s="14">
         <v>11781</v>
       </c>
-      <c r="AV7" s="9">
+      <c r="AV7" s="14">
         <v>12446</v>
       </c>
-      <c r="AW7" s="10">
+      <c r="AW7" s="14">
         <v>12566</v>
       </c>
-      <c r="AX7" s="10"/>
-      <c r="AY7" s="10"/>
-      <c r="AZ7" s="10"/>
-      <c r="BA7" s="10"/>
-      <c r="BB7" s="10"/>
-      <c r="BC7" s="10"/>
-      <c r="BD7" s="10"/>
+      <c r="AX7" s="14"/>
+      <c r="AY7" s="14"/>
+      <c r="AZ7" s="14"/>
+      <c r="BA7" s="14"/>
+      <c r="BB7" s="14"/>
+      <c r="BC7" s="14"/>
+      <c r="BD7" s="14"/>
+      <c r="BE7" s="7"/>
     </row>
-    <row r="8" spans="1:56" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="18">
+    <row r="8" spans="1:110" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
         <v>48</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8">
         <v>12431</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8">
         <v>12139</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8">
         <v>11746</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8">
         <v>10914</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8">
         <v>11094</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8">
         <v>10710</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8">
         <v>10877</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8">
         <v>10795</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8">
         <v>10647</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8">
         <v>10984</v>
       </c>
-      <c r="M8" s="8">
+      <c r="M8">
         <v>10834</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8">
         <v>11401</v>
       </c>
-      <c r="O8" s="8">
+      <c r="O8">
         <v>13787</v>
       </c>
-      <c r="P8" s="8">
+      <c r="P8">
         <v>17897</v>
       </c>
-      <c r="Q8" s="8">
+      <c r="Q8">
         <v>22038</v>
       </c>
-      <c r="R8" s="8">
+      <c r="R8">
         <v>20922</v>
       </c>
-      <c r="S8" s="8">
+      <c r="S8">
         <v>18694</v>
       </c>
-      <c r="T8" s="8">
+      <c r="T8">
         <v>15825</v>
       </c>
-      <c r="U8" s="8">
+      <c r="U8">
         <v>13712</v>
       </c>
-      <c r="V8" s="8">
+      <c r="V8">
         <v>11948</v>
       </c>
-      <c r="W8" s="8">
+      <c r="W8">
         <v>11354</v>
       </c>
-      <c r="X8" s="8">
+      <c r="X8">
         <v>10216</v>
       </c>
-      <c r="Y8" s="8">
+      <c r="Y8">
         <v>9968</v>
       </c>
-      <c r="Z8" s="8">
+      <c r="Z8">
         <v>9454</v>
       </c>
-      <c r="AA8" s="8">
+      <c r="AA8">
         <v>9213</v>
       </c>
-      <c r="AB8" s="8">
+      <c r="AB8">
         <v>9669</v>
       </c>
-      <c r="AC8" s="8">
+      <c r="AC8">
         <v>8745</v>
       </c>
-      <c r="AD8" s="8">
+      <c r="AD8">
         <v>8684</v>
       </c>
-      <c r="AE8" s="8">
+      <c r="AE8" s="14">
         <v>8911</v>
       </c>
-      <c r="AF8" s="8">
+      <c r="AF8" s="14">
         <v>9092</v>
       </c>
-      <c r="AG8" s="8">
+      <c r="AG8" s="14">
         <v>8878</v>
       </c>
-      <c r="AH8" s="8">
+      <c r="AH8" s="14">
         <v>9015</v>
       </c>
-      <c r="AI8" s="8">
+      <c r="AI8" s="14">
         <v>10156</v>
       </c>
-      <c r="AJ8" s="8">
+      <c r="AJ8" s="14">
         <v>8842</v>
       </c>
-      <c r="AK8" s="8">
+      <c r="AK8" s="14">
         <v>8676</v>
       </c>
-      <c r="AL8" s="8">
+      <c r="AL8" s="14">
         <v>9077</v>
       </c>
-      <c r="AM8" s="8">
+      <c r="AM8" s="14">
         <v>9151</v>
       </c>
-      <c r="AN8" s="8">
+      <c r="AN8" s="14">
         <v>9470</v>
       </c>
-      <c r="AO8" s="8">
+      <c r="AO8" s="14">
         <v>9616</v>
       </c>
-      <c r="AP8" s="8">
+      <c r="AP8" s="14">
         <v>9987</v>
       </c>
-      <c r="AQ8" s="8">
+      <c r="AQ8" s="14">
         <v>10348</v>
       </c>
-      <c r="AR8" s="8">
+      <c r="AR8" s="14">
         <v>10385</v>
       </c>
-      <c r="AS8" s="8">
+      <c r="AS8" s="14">
         <v>11098</v>
       </c>
-      <c r="AT8" s="8">
+      <c r="AT8" s="14">
         <v>11446</v>
       </c>
-      <c r="AU8" s="9">
+      <c r="AU8" s="14">
         <v>11797</v>
       </c>
-      <c r="AV8" s="9">
+      <c r="AV8" s="14">
         <v>12391</v>
       </c>
-      <c r="AW8" s="10">
+      <c r="AW8" s="14">
         <v>12391</v>
       </c>
-      <c r="AX8" s="10">
+      <c r="AX8" s="14">
         <v>12471</v>
       </c>
-      <c r="AY8" s="10"/>
-      <c r="AZ8" s="10"/>
-      <c r="BA8" s="10"/>
-      <c r="BB8" s="10"/>
-      <c r="BC8" s="10"/>
-      <c r="BD8" s="10"/>
+      <c r="AY8" s="14"/>
+      <c r="AZ8" s="14"/>
+      <c r="BA8" s="14"/>
+      <c r="BB8" s="14"/>
+      <c r="BC8" s="14"/>
+      <c r="BD8" s="14"/>
+      <c r="BE8" s="7"/>
     </row>
-    <row r="9" spans="1:56" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+    <row r="9" spans="1:110" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
         <v>49</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9">
         <v>12431</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9">
         <v>12139</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9">
         <v>11746</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9">
         <v>10914</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9">
         <v>11094</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9">
         <v>10710</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9">
         <v>10877</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9">
         <v>10795</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9">
         <v>10647</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9">
         <v>10984</v>
       </c>
-      <c r="M9" s="8">
+      <c r="M9">
         <v>10834</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9">
         <v>11401</v>
       </c>
-      <c r="O9" s="8">
+      <c r="O9">
         <v>13787</v>
       </c>
-      <c r="P9" s="8">
+      <c r="P9">
         <v>17897</v>
       </c>
-      <c r="Q9" s="8">
+      <c r="Q9">
         <v>22038</v>
       </c>
-      <c r="R9" s="8">
+      <c r="R9">
         <v>20922</v>
       </c>
-      <c r="S9" s="8">
+      <c r="S9">
         <v>18694</v>
       </c>
-      <c r="T9" s="8">
+      <c r="T9">
         <v>15825</v>
       </c>
-      <c r="U9" s="8">
+      <c r="U9">
         <v>13712</v>
       </c>
-      <c r="V9" s="8">
+      <c r="V9">
         <v>11948</v>
       </c>
-      <c r="W9" s="8">
+      <c r="W9">
         <v>11354</v>
       </c>
-      <c r="X9" s="8">
+      <c r="X9">
         <v>10216</v>
       </c>
-      <c r="Y9" s="8">
+      <c r="Y9">
         <v>9971</v>
       </c>
-      <c r="Z9" s="8">
+      <c r="Z9">
         <v>9456</v>
       </c>
-      <c r="AA9" s="8">
+      <c r="AA9">
         <v>9214</v>
       </c>
-      <c r="AB9" s="8">
+      <c r="AB9">
         <v>9673</v>
       </c>
-      <c r="AC9" s="8">
+      <c r="AC9">
         <v>8747</v>
       </c>
-      <c r="AD9" s="8">
+      <c r="AD9">
         <v>8687</v>
       </c>
-      <c r="AE9" s="8">
+      <c r="AE9" s="14">
         <v>8911</v>
       </c>
-      <c r="AF9" s="8">
+      <c r="AF9" s="14">
         <v>9083</v>
       </c>
-      <c r="AG9" s="8">
+      <c r="AG9" s="14">
         <v>8881</v>
       </c>
-      <c r="AH9" s="8">
+      <c r="AH9" s="14">
         <v>9026</v>
       </c>
-      <c r="AI9" s="8">
+      <c r="AI9" s="14">
         <v>10159</v>
       </c>
-      <c r="AJ9" s="8">
+      <c r="AJ9" s="14">
         <v>8839</v>
       </c>
-      <c r="AK9" s="8">
+      <c r="AK9" s="14">
         <v>8671</v>
       </c>
-      <c r="AL9" s="8">
+      <c r="AL9" s="14">
         <v>9077</v>
       </c>
-      <c r="AM9" s="8">
+      <c r="AM9" s="14">
         <v>9155</v>
       </c>
-      <c r="AN9" s="8">
+      <c r="AN9" s="14">
         <v>9471</v>
       </c>
-      <c r="AO9" s="8">
+      <c r="AO9" s="14">
         <v>9620</v>
       </c>
-      <c r="AP9" s="8">
+      <c r="AP9" s="14">
         <v>9988</v>
       </c>
-      <c r="AQ9" s="8">
+      <c r="AQ9" s="14">
         <v>10355</v>
       </c>
-      <c r="AR9" s="8">
+      <c r="AR9" s="14">
         <v>10381</v>
       </c>
-      <c r="AS9" s="8">
+      <c r="AS9" s="14">
         <v>11098</v>
       </c>
-      <c r="AT9" s="8">
+      <c r="AT9" s="14">
         <v>11450</v>
       </c>
-      <c r="AU9" s="9">
+      <c r="AU9" s="14">
         <v>11790</v>
       </c>
-      <c r="AV9" s="9">
+      <c r="AV9" s="14">
         <v>12395</v>
       </c>
-      <c r="AW9" s="10">
+      <c r="AW9" s="14">
         <v>12367</v>
       </c>
-      <c r="AX9" s="10">
+      <c r="AX9" s="14">
         <v>12382</v>
       </c>
-      <c r="AY9" s="10">
+      <c r="AY9" s="14">
         <v>12155</v>
       </c>
-      <c r="AZ9" s="10"/>
-      <c r="BA9" s="10"/>
-      <c r="BB9" s="10"/>
-      <c r="BC9" s="10"/>
-      <c r="BD9" s="10"/>
+      <c r="AZ9" s="14"/>
+      <c r="BA9" s="14"/>
+      <c r="BB9" s="14"/>
+      <c r="BC9" s="14"/>
+      <c r="BD9" s="14"/>
+      <c r="BE9" s="7"/>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+    <row r="10" spans="1:110" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>50</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="8">
+      <c r="C10">
         <v>12431</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10">
         <v>12139</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10">
         <v>11746</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10">
         <v>10914</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10">
         <v>11094</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10">
         <v>10710</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10">
         <v>10877</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10">
         <v>10795</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10">
         <v>10647</v>
       </c>
-      <c r="L10" s="8">
+      <c r="L10">
         <v>10984</v>
       </c>
-      <c r="M10" s="8">
+      <c r="M10">
         <v>10834</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10">
         <v>11401</v>
       </c>
-      <c r="O10" s="8">
+      <c r="O10">
         <v>13787</v>
       </c>
-      <c r="P10" s="8">
+      <c r="P10">
         <v>17897</v>
       </c>
-      <c r="Q10" s="8">
+      <c r="Q10">
         <v>22038</v>
       </c>
-      <c r="R10" s="8">
+      <c r="R10">
         <v>20922</v>
       </c>
-      <c r="S10" s="8">
+      <c r="S10">
         <v>18694</v>
       </c>
-      <c r="T10" s="8">
+      <c r="T10">
         <v>15825</v>
       </c>
-      <c r="U10" s="8">
+      <c r="U10">
         <v>13712</v>
       </c>
-      <c r="V10" s="8">
+      <c r="V10">
         <v>11948</v>
       </c>
-      <c r="W10" s="8">
+      <c r="W10">
         <v>11354</v>
       </c>
-      <c r="X10" s="8">
+      <c r="X10">
         <v>10216</v>
       </c>
-      <c r="Y10" s="8">
+      <c r="Y10">
         <v>9971</v>
       </c>
-      <c r="Z10" s="8">
+      <c r="Z10">
         <v>9456</v>
       </c>
-      <c r="AA10" s="8">
+      <c r="AA10">
         <v>9214</v>
       </c>
-      <c r="AB10" s="8">
+      <c r="AB10">
         <v>9673</v>
       </c>
-      <c r="AC10" s="8">
+      <c r="AC10">
         <v>8747</v>
       </c>
-      <c r="AD10" s="8">
+      <c r="AD10">
         <v>8687</v>
       </c>
-      <c r="AE10" s="8">
+      <c r="AE10" s="14">
         <v>8898</v>
       </c>
-      <c r="AF10" s="8">
+      <c r="AF10" s="14">
         <v>9079</v>
       </c>
-      <c r="AG10" s="8">
+      <c r="AG10" s="14">
         <v>8877</v>
       </c>
-      <c r="AH10" s="8">
+      <c r="AH10" s="14">
         <v>9021</v>
       </c>
-      <c r="AI10" s="8">
+      <c r="AI10" s="14">
         <v>10155</v>
       </c>
-      <c r="AJ10" s="8">
+      <c r="AJ10" s="14">
         <v>8846</v>
       </c>
-      <c r="AK10" s="8">
+      <c r="AK10" s="14">
         <v>8676</v>
       </c>
-      <c r="AL10" s="8">
+      <c r="AL10" s="14">
         <v>9075</v>
       </c>
-      <c r="AM10" s="8">
+      <c r="AM10" s="14">
         <v>9167</v>
       </c>
-      <c r="AN10" s="8">
+      <c r="AN10" s="14">
         <v>9472</v>
       </c>
-      <c r="AO10" s="8">
+      <c r="AO10" s="14">
         <v>9628</v>
       </c>
-      <c r="AP10" s="8">
+      <c r="AP10" s="14">
         <v>9991</v>
       </c>
-      <c r="AQ10" s="8">
+      <c r="AQ10" s="14">
         <v>10356</v>
       </c>
-      <c r="AR10" s="8">
+      <c r="AR10" s="14">
         <v>10390</v>
       </c>
-      <c r="AS10" s="8">
+      <c r="AS10" s="14">
         <v>11088</v>
       </c>
-      <c r="AT10" s="8">
+      <c r="AT10" s="14">
         <v>11439</v>
       </c>
-      <c r="AU10" s="9">
+      <c r="AU10" s="14">
         <v>11784</v>
       </c>
-      <c r="AV10" s="9">
+      <c r="AV10" s="14">
         <v>12371</v>
       </c>
-      <c r="AW10" s="10">
+      <c r="AW10" s="14">
         <v>12363</v>
       </c>
-      <c r="AX10" s="10">
+      <c r="AX10" s="14">
         <v>12468</v>
       </c>
-      <c r="AY10" s="10">
+      <c r="AY10" s="14">
         <v>12595</v>
       </c>
-      <c r="AZ10" s="10">
+      <c r="AZ10" s="14">
         <v>12097</v>
       </c>
-      <c r="BA10" s="10"/>
-      <c r="BB10" s="10"/>
-      <c r="BC10" s="10"/>
-      <c r="BD10" s="10"/>
+      <c r="BA10" s="14"/>
+      <c r="BB10" s="14"/>
+      <c r="BC10" s="14"/>
+      <c r="BD10" s="14"/>
+      <c r="BE10" s="7"/>
     </row>
-    <row r="11" spans="1:56" s="13" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="12">
+    <row r="11" spans="1:110" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
         <v>51</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11">
         <v>12431</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11">
         <v>12139</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11">
         <v>11746</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11">
         <v>10914</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11">
         <v>11094</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11">
         <v>10710</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11">
         <v>10877</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11">
         <v>10795</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11">
         <v>10647</v>
       </c>
-      <c r="L11" s="8">
+      <c r="L11">
         <v>10984</v>
       </c>
-      <c r="M11" s="8">
+      <c r="M11">
         <v>10834</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11">
         <v>11401</v>
       </c>
-      <c r="O11" s="8">
+      <c r="O11">
         <v>13787</v>
       </c>
-      <c r="P11" s="8">
+      <c r="P11">
         <v>17897</v>
       </c>
-      <c r="Q11" s="8">
+      <c r="Q11">
         <v>22038</v>
       </c>
-      <c r="R11" s="8">
+      <c r="R11">
         <v>20922</v>
       </c>
-      <c r="S11" s="8">
+      <c r="S11">
         <v>18694</v>
       </c>
-      <c r="T11" s="8">
+      <c r="T11">
         <v>15825</v>
       </c>
-      <c r="U11" s="8">
+      <c r="U11">
         <v>13712</v>
       </c>
-      <c r="V11" s="8">
+      <c r="V11">
         <v>11948</v>
       </c>
-      <c r="W11" s="8">
+      <c r="W11">
         <v>11354</v>
       </c>
-      <c r="X11" s="8">
+      <c r="X11">
         <v>10216</v>
       </c>
-      <c r="Y11" s="8">
+      <c r="Y11">
         <v>9971</v>
       </c>
-      <c r="Z11" s="8">
+      <c r="Z11">
         <v>9453</v>
       </c>
-      <c r="AA11" s="8">
+      <c r="AA11">
         <v>9204</v>
       </c>
-      <c r="AB11" s="8">
+      <c r="AB11">
         <v>9671</v>
       </c>
-      <c r="AC11" s="8">
+      <c r="AC11">
         <v>8744</v>
       </c>
-      <c r="AD11" s="8">
+      <c r="AD11">
         <v>8680</v>
       </c>
-      <c r="AE11" s="8">
+      <c r="AE11" s="14">
         <v>8898</v>
       </c>
-      <c r="AF11" s="8">
+      <c r="AF11" s="14">
         <v>9077</v>
       </c>
-      <c r="AG11" s="8">
+      <c r="AG11" s="14">
         <v>8875</v>
       </c>
-      <c r="AH11" s="8">
+      <c r="AH11" s="14">
         <v>9029</v>
       </c>
-      <c r="AI11" s="8">
+      <c r="AI11" s="14">
         <v>10161</v>
       </c>
-      <c r="AJ11" s="8">
+      <c r="AJ11" s="14">
         <v>8848</v>
       </c>
-      <c r="AK11" s="8">
+      <c r="AK11" s="14">
         <v>8675</v>
       </c>
-      <c r="AL11" s="8">
+      <c r="AL11" s="14">
         <v>9081</v>
       </c>
-      <c r="AM11" s="8">
+      <c r="AM11" s="14">
         <v>9169</v>
       </c>
-      <c r="AN11" s="8">
+      <c r="AN11" s="14">
         <v>9468</v>
       </c>
-      <c r="AO11" s="8">
+      <c r="AO11" s="14">
         <v>9626</v>
       </c>
-      <c r="AP11" s="8">
+      <c r="AP11" s="14">
         <v>9992</v>
       </c>
-      <c r="AQ11" s="8">
+      <c r="AQ11" s="14">
         <v>10358</v>
       </c>
-      <c r="AR11" s="8">
+      <c r="AR11" s="14">
         <v>10393</v>
       </c>
-      <c r="AS11" s="8">
+      <c r="AS11" s="14">
         <v>11092</v>
       </c>
-      <c r="AT11" s="8">
+      <c r="AT11" s="14">
         <v>11438</v>
       </c>
-      <c r="AU11" s="9">
+      <c r="AU11" s="14">
         <v>11794</v>
       </c>
-      <c r="AV11" s="9">
+      <c r="AV11" s="14">
         <v>12373</v>
       </c>
-      <c r="AW11" s="10">
+      <c r="AW11" s="14">
         <v>12350</v>
       </c>
-      <c r="AX11" s="10">
+      <c r="AX11" s="14">
         <v>12483</v>
       </c>
-      <c r="AY11" s="10">
+      <c r="AY11" s="14">
         <v>12673</v>
       </c>
-      <c r="AZ11" s="10">
+      <c r="AZ11" s="14">
         <v>12999</v>
       </c>
-      <c r="BA11" s="10">
+      <c r="BA11" s="14">
         <v>13097</v>
       </c>
-      <c r="BB11" s="10"/>
-      <c r="BC11" s="10"/>
-      <c r="BD11" s="10"/>
+      <c r="BB11" s="14"/>
+      <c r="BC11" s="14"/>
+      <c r="BD11" s="14"/>
+      <c r="BE11" s="7"/>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
+    <row r="12" spans="1:110" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
         <v>52</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="8">
+      <c r="B12" s="9"/>
+      <c r="C12" s="7">
         <v>12431</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <v>12139</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>11746</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <v>10914</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>11094</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="7">
         <v>10710</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="7">
         <v>10877</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="7">
         <v>10795</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12" s="7">
         <v>10647</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L12" s="7">
         <v>10984</v>
       </c>
-      <c r="M12" s="8">
+      <c r="M12" s="7">
         <v>10834</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12" s="7">
         <v>11401</v>
       </c>
-      <c r="O12" s="8">
+      <c r="O12" s="7">
         <v>13787</v>
       </c>
-      <c r="P12" s="8">
+      <c r="P12" s="7">
         <v>17897</v>
       </c>
-      <c r="Q12" s="8">
+      <c r="Q12" s="7">
         <v>22038</v>
       </c>
-      <c r="R12" s="8">
+      <c r="R12" s="7">
         <v>20922</v>
       </c>
-      <c r="S12" s="8">
+      <c r="S12" s="7">
         <v>18694</v>
       </c>
-      <c r="T12" s="8">
+      <c r="T12" s="7">
         <v>15825</v>
       </c>
-      <c r="U12" s="8">
+      <c r="U12" s="7">
         <v>13712</v>
       </c>
-      <c r="V12" s="8">
+      <c r="V12" s="7">
         <v>11948</v>
       </c>
-      <c r="W12" s="8">
+      <c r="W12" s="7">
         <v>11354</v>
       </c>
-      <c r="X12" s="8">
+      <c r="X12" s="7">
         <v>10216</v>
       </c>
-      <c r="Y12" s="8">
+      <c r="Y12" s="7">
         <v>9971</v>
       </c>
-      <c r="Z12" s="8">
+      <c r="Z12" s="7">
         <v>9453</v>
       </c>
-      <c r="AA12" s="8">
+      <c r="AA12" s="7">
         <v>9204</v>
       </c>
-      <c r="AB12" s="8">
+      <c r="AB12" s="7">
         <v>9661</v>
       </c>
-      <c r="AC12" s="8">
+      <c r="AC12" s="7">
         <v>8740</v>
       </c>
-      <c r="AD12" s="8">
+      <c r="AD12" s="7">
         <v>8680</v>
       </c>
-      <c r="AE12" s="8">
+      <c r="AE12" s="7">
         <v>8893</v>
       </c>
-      <c r="AF12" s="8">
+      <c r="AF12" s="7">
         <v>9070</v>
       </c>
-      <c r="AG12" s="8">
+      <c r="AG12" s="7">
         <v>8871</v>
       </c>
-      <c r="AH12" s="8">
+      <c r="AH12" s="7">
         <v>9023</v>
       </c>
-      <c r="AI12" s="8">
+      <c r="AI12" s="7">
         <v>10154</v>
       </c>
-      <c r="AJ12" s="8">
+      <c r="AJ12" s="7">
         <v>8853</v>
       </c>
-      <c r="AK12" s="8">
+      <c r="AK12" s="7">
         <v>8673</v>
       </c>
-      <c r="AL12" s="8">
+      <c r="AL12" s="7">
         <v>9084</v>
       </c>
-      <c r="AM12" s="8">
+      <c r="AM12" s="7">
         <v>9159</v>
       </c>
-      <c r="AN12" s="8">
+      <c r="AN12" s="7">
         <v>9463</v>
       </c>
-      <c r="AO12" s="8">
+      <c r="AO12" s="7">
         <v>9621</v>
       </c>
-      <c r="AP12" s="8">
+      <c r="AP12" s="7">
         <v>9987</v>
       </c>
-      <c r="AQ12" s="8">
+      <c r="AQ12" s="7">
         <v>10351</v>
       </c>
-      <c r="AR12" s="8">
+      <c r="AR12" s="7">
         <v>10392</v>
       </c>
-      <c r="AS12" s="8">
+      <c r="AS12" s="7">
         <v>11078</v>
       </c>
-      <c r="AT12" s="8">
+      <c r="AT12" s="14">
         <v>11431</v>
       </c>
-      <c r="AU12" s="9">
+      <c r="AU12" s="14">
         <v>11788</v>
       </c>
-      <c r="AV12" s="9">
+      <c r="AV12" s="14">
         <v>12370</v>
       </c>
-      <c r="AW12" s="10">
+      <c r="AW12" s="14">
         <v>12338</v>
       </c>
-      <c r="AX12" s="10">
+      <c r="AX12" s="14">
         <v>12456</v>
       </c>
-      <c r="AY12" s="10">
+      <c r="AY12" s="14">
         <v>12675</v>
       </c>
-      <c r="AZ12" s="10">
+      <c r="AZ12" s="14">
         <v>13037</v>
       </c>
-      <c r="BA12" s="10">
+      <c r="BA12" s="14">
         <v>13197</v>
       </c>
-      <c r="BB12" s="24">
+      <c r="BB12" s="14">
         <v>14439</v>
       </c>
-      <c r="BC12" s="24"/>
-      <c r="BD12" s="10"/>
+      <c r="BC12" s="14"/>
+      <c r="BD12" s="7"/>
+      <c r="BE12" s="7"/>
+      <c r="BF12" s="7"/>
+      <c r="BG12" s="7"/>
+      <c r="BH12" s="7"/>
+      <c r="BI12" s="7"/>
+      <c r="BJ12" s="7"/>
+      <c r="BK12" s="7"/>
+      <c r="BL12" s="7"/>
+      <c r="BM12" s="7"/>
+      <c r="BN12" s="7"/>
+      <c r="BO12" s="7"/>
+      <c r="BP12" s="7"/>
+      <c r="BQ12" s="7"/>
+      <c r="BR12" s="7"/>
+      <c r="BS12" s="7"/>
+      <c r="BT12" s="7"/>
+      <c r="BU12" s="7"/>
+      <c r="BV12" s="7"/>
+      <c r="BW12" s="7"/>
+      <c r="BX12" s="7"/>
+      <c r="BY12" s="7"/>
+      <c r="BZ12" s="7"/>
+      <c r="CA12" s="7"/>
+      <c r="CB12" s="7"/>
+      <c r="CC12" s="7"/>
+      <c r="CD12" s="7"/>
+      <c r="CE12" s="7"/>
+      <c r="CF12" s="7"/>
+      <c r="CG12" s="7"/>
+      <c r="CH12" s="7"/>
+      <c r="CI12" s="7"/>
+      <c r="CJ12" s="7"/>
+      <c r="CK12" s="7"/>
+      <c r="CL12" s="7"/>
+      <c r="CM12" s="7"/>
+      <c r="CN12" s="7"/>
+      <c r="CO12" s="7"/>
+      <c r="CP12" s="7"/>
+      <c r="CQ12" s="7"/>
+      <c r="CR12" s="7"/>
+      <c r="CS12" s="7"/>
+      <c r="CT12" s="7"/>
+      <c r="CU12" s="7"/>
+      <c r="CV12" s="7"/>
+      <c r="CW12" s="7"/>
+      <c r="CX12" s="7"/>
+      <c r="CY12" s="7"/>
+      <c r="CZ12" s="7"/>
+      <c r="DA12" s="7"/>
+      <c r="DB12" s="7"/>
+      <c r="DC12" s="7"/>
+      <c r="DD12" s="7"/>
+      <c r="DE12" s="7"/>
+      <c r="DF12" s="7"/>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
+    <row r="13" spans="1:110" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
         <v>53</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="8">
+      <c r="B13" s="9"/>
+      <c r="C13" s="7">
         <v>12431</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <v>12139</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <v>11746</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <v>10914</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>11094</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="7">
         <v>10710</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <v>10877</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="7">
         <v>10795</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="7">
         <v>10647</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="7">
         <v>10984</v>
       </c>
-      <c r="M13" s="8">
+      <c r="M13" s="7">
         <v>10834</v>
       </c>
-      <c r="N13" s="8">
+      <c r="N13" s="7">
         <v>11401</v>
       </c>
-      <c r="O13" s="8">
+      <c r="O13" s="7">
         <v>13787</v>
       </c>
-      <c r="P13" s="8">
+      <c r="P13" s="7">
         <v>17897</v>
       </c>
-      <c r="Q13" s="8">
+      <c r="Q13" s="7">
         <v>22038</v>
       </c>
-      <c r="R13" s="8">
+      <c r="R13" s="7">
         <v>20922</v>
       </c>
-      <c r="S13" s="8">
+      <c r="S13" s="7">
         <v>18694</v>
       </c>
-      <c r="T13" s="8">
+      <c r="T13" s="7">
         <v>15825</v>
       </c>
-      <c r="U13" s="8">
+      <c r="U13" s="7">
         <v>13712</v>
       </c>
-      <c r="V13" s="8">
+      <c r="V13" s="7">
         <v>11948</v>
       </c>
-      <c r="W13" s="8">
+      <c r="W13" s="7">
         <v>11354</v>
       </c>
-      <c r="X13" s="8">
+      <c r="X13" s="7">
         <v>10216</v>
       </c>
-      <c r="Y13" s="8">
+      <c r="Y13" s="7">
         <v>9971</v>
       </c>
-      <c r="Z13" s="8">
+      <c r="Z13" s="7">
         <v>9453</v>
       </c>
-      <c r="AA13" s="8">
+      <c r="AA13" s="7">
         <v>9204</v>
       </c>
-      <c r="AB13" s="8">
+      <c r="AB13" s="7">
         <v>9661</v>
       </c>
-      <c r="AC13" s="8">
+      <c r="AC13" s="7">
         <v>8740</v>
       </c>
-      <c r="AD13" s="8">
+      <c r="AD13" s="7">
         <v>8680</v>
       </c>
-      <c r="AE13" s="8">
+      <c r="AE13" s="7">
         <v>8893</v>
       </c>
-      <c r="AF13" s="8">
+      <c r="AF13" s="7">
         <v>9070</v>
       </c>
-      <c r="AG13" s="8">
+      <c r="AG13" s="7">
         <v>8871</v>
       </c>
-      <c r="AH13" s="8">
+      <c r="AH13" s="7">
         <v>9023</v>
       </c>
-      <c r="AI13" s="8">
+      <c r="AI13" s="7">
         <v>10154</v>
       </c>
-      <c r="AJ13" s="8">
+      <c r="AJ13" s="7">
         <v>8853</v>
       </c>
-      <c r="AK13" s="8">
+      <c r="AK13" s="7">
         <v>8673</v>
       </c>
-      <c r="AL13" s="8">
+      <c r="AL13" s="7">
         <v>9084</v>
       </c>
-      <c r="AM13" s="8">
+      <c r="AM13" s="7">
         <v>9159</v>
       </c>
-      <c r="AN13" s="8">
+      <c r="AN13" s="7">
         <v>9463</v>
       </c>
-      <c r="AO13" s="8">
+      <c r="AO13" s="7">
         <v>9621</v>
       </c>
-      <c r="AP13" s="8">
+      <c r="AP13" s="7">
         <v>9987</v>
       </c>
-      <c r="AQ13" s="8">
+      <c r="AQ13" s="7">
         <v>10351</v>
       </c>
-      <c r="AR13" s="8">
+      <c r="AR13" s="7">
         <v>10392</v>
       </c>
-      <c r="AS13" s="8">
+      <c r="AS13" s="7">
         <v>11078</v>
       </c>
-      <c r="AT13" s="8">
+      <c r="AT13" s="14">
         <v>11431</v>
       </c>
-      <c r="AU13" s="9">
+      <c r="AU13" s="14">
         <v>11788</v>
       </c>
-      <c r="AV13" s="9">
+      <c r="AV13" s="14">
         <v>12370</v>
       </c>
-      <c r="AW13" s="20">
+      <c r="AW13" s="14">
         <v>12338</v>
       </c>
-      <c r="AX13" s="20">
+      <c r="AX13" s="14">
         <v>12456</v>
       </c>
-      <c r="AY13" s="20">
+      <c r="AY13" s="14">
         <v>12675</v>
       </c>
-      <c r="AZ13" s="20">
+      <c r="AZ13" s="14">
         <v>13037</v>
       </c>
-      <c r="BA13" s="20">
+      <c r="BA13" s="14">
         <v>13197</v>
       </c>
-      <c r="BB13" s="25">
+      <c r="BB13" s="11">
         <v>14439</v>
       </c>
-      <c r="BC13" s="25"/>
-      <c r="BD13" s="10"/>
+      <c r="BC13" s="12"/>
+      <c r="BD13" s="7"/>
+      <c r="BE13" s="7"/>
+      <c r="BF13" s="7"/>
+      <c r="BG13" s="7"/>
+      <c r="BH13" s="7"/>
+      <c r="BI13" s="7"/>
+      <c r="BJ13" s="7"/>
+      <c r="BK13" s="7"/>
+      <c r="BL13" s="7"/>
+      <c r="BM13" s="7"/>
+      <c r="BN13" s="7"/>
+      <c r="BO13" s="7"/>
+      <c r="BP13" s="7"/>
+      <c r="BQ13" s="7"/>
+      <c r="BR13" s="7"/>
+      <c r="BS13" s="7"/>
+      <c r="BT13" s="7"/>
+      <c r="BU13" s="7"/>
+      <c r="BV13" s="7"/>
+      <c r="BW13" s="7"/>
+      <c r="BX13" s="7"/>
+      <c r="BY13" s="7"/>
+      <c r="BZ13" s="7"/>
+      <c r="CA13" s="7"/>
+      <c r="CB13" s="7"/>
+      <c r="CC13" s="7"/>
+      <c r="CD13" s="7"/>
+      <c r="CE13" s="7"/>
+      <c r="CF13" s="7"/>
+      <c r="CG13" s="7"/>
+      <c r="CH13" s="7"/>
+      <c r="CI13" s="7"/>
+      <c r="CJ13" s="7"/>
+      <c r="CK13" s="7"/>
+      <c r="CL13" s="7"/>
+      <c r="CM13" s="7"/>
+      <c r="CN13" s="7"/>
+      <c r="CO13" s="7"/>
+      <c r="CP13" s="7"/>
+      <c r="CQ13" s="7"/>
+      <c r="CR13" s="7"/>
+      <c r="CS13" s="7"/>
+      <c r="CT13" s="7"/>
+      <c r="CU13" s="7"/>
+      <c r="CV13" s="7"/>
+      <c r="CW13" s="7"/>
+      <c r="CX13" s="7"/>
+      <c r="CY13" s="7"/>
+      <c r="CZ13" s="7"/>
+      <c r="DA13" s="7"/>
+      <c r="DB13" s="7"/>
+      <c r="DC13" s="7"/>
+      <c r="DD13" s="7"/>
+      <c r="DE13" s="7"/>
+      <c r="DF13" s="7"/>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
+    <row r="14" spans="1:110" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
         <v>1</v>
       </c>
-      <c r="AD14" s="23">
+      <c r="AD14" s="10">
         <v>8662</v>
       </c>
-      <c r="AE14" s="23">
+      <c r="AE14" s="10">
         <v>8877</v>
       </c>
-      <c r="AF14" s="23">
+      <c r="AF14" s="10">
         <v>9048</v>
       </c>
-      <c r="AG14" s="23">
+      <c r="AG14" s="10">
         <v>8860</v>
       </c>
-      <c r="AH14" s="23">
+      <c r="AH14" s="10">
         <v>9010</v>
       </c>
-      <c r="AI14" s="23">
+      <c r="AI14" s="10">
         <v>10130</v>
       </c>
-      <c r="AJ14" s="23">
+      <c r="AJ14" s="10">
         <v>8829</v>
       </c>
-      <c r="AK14" s="23">
+      <c r="AK14" s="10">
         <v>8652</v>
       </c>
-      <c r="AL14" s="23">
+      <c r="AL14" s="10">
         <v>9053</v>
       </c>
-      <c r="AM14" s="23">
+      <c r="AM14" s="10">
         <v>9136</v>
       </c>
-      <c r="AN14" s="23">
+      <c r="AN14" s="10">
         <v>9433</v>
       </c>
-      <c r="AO14" s="23">
+      <c r="AO14" s="10">
         <v>9598</v>
       </c>
-      <c r="AP14" s="23">
+      <c r="AP14" s="10">
         <v>9965</v>
       </c>
-      <c r="AQ14" s="23">
+      <c r="AQ14" s="10">
         <v>10324</v>
       </c>
-      <c r="AR14" s="23">
+      <c r="AR14" s="10">
         <v>10368</v>
       </c>
-      <c r="AS14" s="23">
+      <c r="AS14" s="10">
         <v>11058</v>
       </c>
-      <c r="AT14" s="23">
+      <c r="AT14" s="14">
         <v>11402</v>
       </c>
-      <c r="AU14" s="23">
+      <c r="AU14" s="14">
         <v>11757</v>
       </c>
-      <c r="AV14" s="23">
+      <c r="AV14" s="14">
         <v>12347</v>
       </c>
-      <c r="AW14" s="23">
+      <c r="AW14" s="14">
         <v>12316</v>
       </c>
-      <c r="AX14" s="23">
+      <c r="AX14" s="14">
         <v>12429</v>
       </c>
-      <c r="AY14" s="23">
+      <c r="AY14" s="14">
         <v>12640</v>
       </c>
-      <c r="AZ14" s="23">
+      <c r="AZ14" s="14">
         <v>13009</v>
       </c>
-      <c r="BA14" s="23">
+      <c r="BA14" s="14">
         <v>13085</v>
       </c>
-      <c r="BB14" s="23">
+      <c r="BB14" s="10">
         <v>13281</v>
       </c>
-      <c r="BC14" s="26">
+      <c r="BC14" s="15">
         <f>(BB14+BD14)/2</f>
         <v>14484</v>
       </c>
-      <c r="BD14" s="23">
+      <c r="BD14" s="10">
         <v>15687</v>
+      </c>
+    </row>
+    <row r="15" spans="1:110" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>2</v>
+      </c>
+      <c r="AE15" s="14">
+        <v>8874</v>
+      </c>
+      <c r="AF15" s="14">
+        <v>9044</v>
+      </c>
+      <c r="AG15" s="14">
+        <v>8851</v>
+      </c>
+      <c r="AH15" s="14">
+        <v>9011</v>
+      </c>
+      <c r="AI15" s="14">
+        <v>10137</v>
+      </c>
+      <c r="AJ15" s="14">
+        <v>8829</v>
+      </c>
+      <c r="AK15" s="14">
+        <v>8652</v>
+      </c>
+      <c r="AL15" s="14">
+        <v>9048</v>
+      </c>
+      <c r="AM15" s="14">
+        <v>9135</v>
+      </c>
+      <c r="AN15" s="14">
+        <v>9440</v>
+      </c>
+      <c r="AO15" s="14">
+        <v>9594</v>
+      </c>
+      <c r="AP15" s="14">
+        <v>9967</v>
+      </c>
+      <c r="AQ15" s="14">
+        <v>10323</v>
+      </c>
+      <c r="AR15" s="14">
+        <v>10368</v>
+      </c>
+      <c r="AS15" s="14">
+        <v>11062</v>
+      </c>
+      <c r="AT15" s="14">
+        <v>11393</v>
+      </c>
+      <c r="AU15" s="14">
+        <v>11755</v>
+      </c>
+      <c r="AV15" s="14">
+        <v>12348</v>
+      </c>
+      <c r="AW15" s="14">
+        <v>12313</v>
+      </c>
+      <c r="AX15" s="14">
+        <v>12443</v>
+      </c>
+      <c r="AY15" s="14">
+        <v>12656</v>
+      </c>
+      <c r="AZ15" s="14">
+        <v>13017</v>
+      </c>
+      <c r="BA15" s="14">
+        <v>13140</v>
+      </c>
+      <c r="BB15" s="14">
+        <v>13413</v>
+      </c>
+      <c r="BC15" s="14">
+        <v>14747</v>
+      </c>
+      <c r="BD15" s="14">
+        <v>16645</v>
+      </c>
+      <c r="BE15" s="7">
+        <v>20004</v>
       </c>
     </row>
   </sheetData>
@@ -5568,67 +5912,67 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB243748-DFB5-4F65-A856-C18F501810ED}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B26"/>
+      <selection activeCell="B2" sqref="B2:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6">
-        <v>44022</v>
-      </c>
-      <c r="B1" s="23">
-        <v>8662</v>
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>44029</v>
       </c>
-      <c r="B2" s="23">
-        <v>8877</v>
+      <c r="B2" s="14">
+        <v>8874</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>44036</v>
       </c>
-      <c r="B3" s="23">
-        <v>9048</v>
+      <c r="B3" s="14">
+        <v>9044</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>44043</v>
       </c>
-      <c r="B4" s="23">
-        <v>8860</v>
+      <c r="B4" s="14">
+        <v>8851</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>44050</v>
       </c>
-      <c r="B5" s="23">
-        <v>9010</v>
+      <c r="B5" s="14">
+        <v>9011</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>44057</v>
       </c>
-      <c r="B6" s="23">
-        <v>10130</v>
+      <c r="B6" s="14">
+        <v>10137</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>44064</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="14">
         <v>8829</v>
       </c>
     </row>
@@ -5636,7 +5980,7 @@
       <c r="A8" s="6">
         <v>44071</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="14">
         <v>8652</v>
       </c>
     </row>
@@ -5644,55 +5988,55 @@
       <c r="A9" s="6">
         <v>44078</v>
       </c>
-      <c r="B9" s="23">
-        <v>9053</v>
+      <c r="B9" s="14">
+        <v>9048</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>44085</v>
       </c>
-      <c r="B10" s="23">
-        <v>9136</v>
+      <c r="B10" s="14">
+        <v>9135</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>44092</v>
       </c>
-      <c r="B11" s="23">
-        <v>9433</v>
+      <c r="B11" s="14">
+        <v>9440</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>44099</v>
       </c>
-      <c r="B12" s="23">
-        <v>9598</v>
+      <c r="B12" s="14">
+        <v>9594</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>44106</v>
       </c>
-      <c r="B13" s="23">
-        <v>9965</v>
+      <c r="B13" s="14">
+        <v>9967</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>44113</v>
       </c>
-      <c r="B14" s="23">
-        <v>10324</v>
+      <c r="B14" s="14">
+        <v>10323</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>44120</v>
       </c>
-      <c r="B15" s="23">
+      <c r="B15" s="14">
         <v>10368</v>
       </c>
     </row>
@@ -5700,93 +6044,109 @@
       <c r="A16" s="6">
         <v>44127</v>
       </c>
-      <c r="B16" s="23">
-        <v>11058</v>
+      <c r="B16" s="14">
+        <v>11062</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>44134</v>
       </c>
-      <c r="B17" s="23">
-        <v>11402</v>
+      <c r="B17" s="14">
+        <v>11393</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>44141</v>
       </c>
-      <c r="B18" s="23">
-        <v>11757</v>
+      <c r="B18" s="14">
+        <v>11755</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>44148</v>
       </c>
-      <c r="B19" s="23">
-        <v>12347</v>
+      <c r="B19" s="14">
+        <v>12348</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>44155</v>
       </c>
-      <c r="B20" s="23">
-        <v>12316</v>
+      <c r="B20" s="14">
+        <v>12313</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>44162</v>
       </c>
-      <c r="B21" s="23">
-        <v>12429</v>
+      <c r="B21" s="14">
+        <v>12443</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>44169</v>
       </c>
-      <c r="B22" s="23">
-        <v>12640</v>
+      <c r="B22" s="14">
+        <v>12656</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>44176</v>
       </c>
-      <c r="B23" s="23">
-        <v>13009</v>
+      <c r="B23" s="14">
+        <v>13017</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>44183</v>
       </c>
-      <c r="B24" s="23">
-        <v>13085</v>
+      <c r="B24" s="14">
+        <v>13140</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>44190</v>
       </c>
-      <c r="B25" s="23">
-        <v>13281</v>
+      <c r="B25" s="14">
+        <v>13413</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
+        <v>44197</v>
+      </c>
+      <c r="B26" s="14">
+        <v>14747</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
         <v>44204</v>
       </c>
-      <c r="B26" s="23">
-        <v>15687</v>
+      <c r="B27" s="14">
+        <v>16645</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>44211</v>
+      </c>
+      <c r="B28" s="13">
+        <v>20004</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B26">
-    <sortCondition ref="A1:A26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B27">
+    <sortCondition ref="A2:A27"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5797,7 +6157,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Refresh evaluation of ONS estimates
</commit_message>
<xml_diff>
--- a/data/ons-deaths/explore/evaluation_of_ons_estimates.xlsx
+++ b/data/ons-deaths/explore/evaluation_of_ons_estimates.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\covid-stats\data\ons-deaths\explore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EDF98B-F2E2-41EC-A5FA-DCB4F8D88D61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB786113-A367-4DB0-9544-05A0B5AFDB03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{A515F7DA-6FDB-438E-B4AB-3C334154F930}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{A515F7DA-6FDB-438E-B4AB-3C334154F930}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="pivot" sheetId="2" r:id="rId2"/>
-    <sheet name="chart" sheetId="3" r:id="rId3"/>
+    <sheet name="chart" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,18 +26,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Week number</t>
   </si>
   <si>
     <t>Week ended</t>
-  </si>
-  <si>
-    <t>week ended</t>
-  </si>
-  <si>
-    <t>estimate</t>
   </si>
 </sst>
 </file>
@@ -605,7 +598,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -642,6 +635,9 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1186,6 +1182,15 @@
                 <c:pt idx="12">
                   <c:v>44211</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>44218</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44225</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44232</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1278,6 +1283,15 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44211</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44218</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44225</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44232</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1377,6 +1391,15 @@
                 <c:pt idx="12">
                   <c:v>44211</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>44218</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44225</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44232</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1476,6 +1499,15 @@
                 <c:pt idx="12">
                   <c:v>44211</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>44218</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44225</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44232</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1578,6 +1610,15 @@
                 <c:pt idx="12">
                   <c:v>44211</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>44218</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44225</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44232</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1683,6 +1724,15 @@
                 <c:pt idx="12">
                   <c:v>44211</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>44218</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44225</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44232</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1790,6 +1840,15 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44211</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44218</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44225</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44232</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1904,6 +1963,15 @@
                 <c:pt idx="12">
                   <c:v>44211</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>44218</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44225</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44232</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2020,6 +2088,15 @@
                 <c:pt idx="12">
                   <c:v>44211</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>44218</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44225</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44232</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2139,6 +2216,15 @@
                 <c:pt idx="12">
                   <c:v>44211</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>44218</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44225</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44232</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2261,6 +2347,15 @@
                 <c:pt idx="12">
                   <c:v>44211</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>44218</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44225</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44232</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2389,6 +2484,15 @@
                 <c:pt idx="12">
                   <c:v>44211</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>44218</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44225</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44232</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2444,6 +2548,276 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-D9F9-4C3B-AA97-5A99ABF51506}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3 </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AS$16:$ZZ$16</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="658"/>
+                <c:pt idx="0">
+                  <c:v>11055</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11392</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11754</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12351</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12314</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12448</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12662</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13043</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13158</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13481</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14932</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16253</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18619</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19288</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C0CA-4F4D-8A7E-8BBD1C545922}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4 </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AS$17:$ZZ$17</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="658"/>
+                <c:pt idx="0">
+                  <c:v>11052</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11398</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11750</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12346</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12324</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12452</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12661</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13045</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13166</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13498</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14990</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16456</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18465</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19435</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17827</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-C0CA-4F4D-8A7E-8BBD1C545922}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="14"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5 </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AS$18:$ZZ$18</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="658"/>
+                <c:pt idx="0">
+                  <c:v>11045</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11391</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11748</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12343</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12329</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12451</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12658</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13043</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13168</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13504</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16491</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18629</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19300</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18048</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16470</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-C0CA-4F4D-8A7E-8BBD1C545922}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3545,13 +3919,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D1BBA0-D981-49C0-9749-BCE3B566D49F}">
-  <dimension ref="A1:DF15"/>
+  <dimension ref="A1:DF20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="AS3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BC16" sqref="BC16"/>
+      <selection pane="bottomRight" activeCell="BK16" sqref="BK16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3735,6 +4109,18 @@
       <c r="BD1" s="3">
         <v>1</v>
       </c>
+      <c r="BE1" s="2">
+        <v>2</v>
+      </c>
+      <c r="BF1" s="3">
+        <v>3</v>
+      </c>
+      <c r="BG1" s="2">
+        <v>4</v>
+      </c>
+      <c r="BH1" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="1:110" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -3905,6 +4291,15 @@
       </c>
       <c r="BE2" s="6">
         <v>44211</v>
+      </c>
+      <c r="BF2" s="6">
+        <v>44218</v>
+      </c>
+      <c r="BG2" s="6">
+        <v>44225</v>
+      </c>
+      <c r="BH2" s="6">
+        <v>44232</v>
       </c>
     </row>
     <row r="3" spans="1:110" x14ac:dyDescent="0.25">
@@ -5902,262 +6297,286 @@
         <v>20004</v>
       </c>
     </row>
+    <row r="16" spans="1:110" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>3</v>
+      </c>
+      <c r="AE16" s="14">
+        <v>8874</v>
+      </c>
+      <c r="AF16" s="14">
+        <v>9050</v>
+      </c>
+      <c r="AG16" s="14">
+        <v>8854</v>
+      </c>
+      <c r="AH16" s="14">
+        <v>9007</v>
+      </c>
+      <c r="AI16" s="14">
+        <v>10142</v>
+      </c>
+      <c r="AJ16" s="14">
+        <v>8831</v>
+      </c>
+      <c r="AK16" s="14">
+        <v>8650</v>
+      </c>
+      <c r="AL16" s="14">
+        <v>9053</v>
+      </c>
+      <c r="AM16" s="14">
+        <v>9129</v>
+      </c>
+      <c r="AN16" s="14">
+        <v>9443</v>
+      </c>
+      <c r="AO16" s="14">
+        <v>9584</v>
+      </c>
+      <c r="AP16" s="14">
+        <v>9973</v>
+      </c>
+      <c r="AQ16" s="14">
+        <v>10325</v>
+      </c>
+      <c r="AR16" s="14">
+        <v>10382</v>
+      </c>
+      <c r="AS16" s="14">
+        <v>11055</v>
+      </c>
+      <c r="AT16" s="14">
+        <v>11392</v>
+      </c>
+      <c r="AU16" s="14">
+        <v>11754</v>
+      </c>
+      <c r="AV16" s="14">
+        <v>12351</v>
+      </c>
+      <c r="AW16" s="14">
+        <v>12314</v>
+      </c>
+      <c r="AX16" s="14">
+        <v>12448</v>
+      </c>
+      <c r="AY16" s="14">
+        <v>12662</v>
+      </c>
+      <c r="AZ16" s="14">
+        <v>13043</v>
+      </c>
+      <c r="BA16" s="14">
+        <v>13158</v>
+      </c>
+      <c r="BB16" s="14">
+        <v>13481</v>
+      </c>
+      <c r="BC16" s="14">
+        <v>14932</v>
+      </c>
+      <c r="BD16" s="14">
+        <v>16253</v>
+      </c>
+      <c r="BE16" s="13">
+        <v>18619</v>
+      </c>
+      <c r="BF16" s="10">
+        <v>19288</v>
+      </c>
+    </row>
+    <row r="17" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>4</v>
+      </c>
+      <c r="AF17" s="14"/>
+      <c r="AG17" s="14">
+        <v>8852</v>
+      </c>
+      <c r="AH17" s="14">
+        <v>9010</v>
+      </c>
+      <c r="AI17" s="14">
+        <v>10142</v>
+      </c>
+      <c r="AJ17" s="14">
+        <v>8830</v>
+      </c>
+      <c r="AK17" s="14">
+        <v>8650</v>
+      </c>
+      <c r="AL17" s="14">
+        <v>9048</v>
+      </c>
+      <c r="AM17" s="14">
+        <v>9134</v>
+      </c>
+      <c r="AN17" s="14">
+        <v>9447</v>
+      </c>
+      <c r="AO17" s="14">
+        <v>9588</v>
+      </c>
+      <c r="AP17" s="14">
+        <v>9968</v>
+      </c>
+      <c r="AQ17" s="14">
+        <v>10324</v>
+      </c>
+      <c r="AR17" s="14">
+        <v>10382</v>
+      </c>
+      <c r="AS17" s="14">
+        <v>11052</v>
+      </c>
+      <c r="AT17" s="14">
+        <v>11398</v>
+      </c>
+      <c r="AU17" s="14">
+        <v>11750</v>
+      </c>
+      <c r="AV17" s="14">
+        <v>12346</v>
+      </c>
+      <c r="AW17" s="14">
+        <v>12324</v>
+      </c>
+      <c r="AX17" s="14">
+        <v>12452</v>
+      </c>
+      <c r="AY17" s="14">
+        <v>12661</v>
+      </c>
+      <c r="AZ17" s="14">
+        <v>13045</v>
+      </c>
+      <c r="BA17" s="14">
+        <v>13166</v>
+      </c>
+      <c r="BB17" s="14">
+        <v>13498</v>
+      </c>
+      <c r="BC17" s="14">
+        <v>14990</v>
+      </c>
+      <c r="BD17" s="14">
+        <v>16456</v>
+      </c>
+      <c r="BE17" s="14">
+        <v>18465</v>
+      </c>
+      <c r="BF17" s="13">
+        <v>19435</v>
+      </c>
+      <c r="BG17" s="10">
+        <v>17827</v>
+      </c>
+      <c r="BH17" s="10"/>
+    </row>
+    <row r="18" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>5</v>
+      </c>
+      <c r="AF18" s="14"/>
+      <c r="AG18" s="14"/>
+      <c r="AH18" s="14">
+        <v>9008</v>
+      </c>
+      <c r="AI18" s="14">
+        <v>10141</v>
+      </c>
+      <c r="AJ18" s="14">
+        <v>8831</v>
+      </c>
+      <c r="AK18" s="14">
+        <v>8658</v>
+      </c>
+      <c r="AL18" s="14">
+        <v>9044</v>
+      </c>
+      <c r="AM18" s="14">
+        <v>9145</v>
+      </c>
+      <c r="AN18" s="14">
+        <v>9457</v>
+      </c>
+      <c r="AO18" s="14">
+        <v>9587</v>
+      </c>
+      <c r="AP18" s="14">
+        <v>9966</v>
+      </c>
+      <c r="AQ18" s="14">
+        <v>10319</v>
+      </c>
+      <c r="AR18" s="14">
+        <v>10379</v>
+      </c>
+      <c r="AS18" s="14">
+        <v>11045</v>
+      </c>
+      <c r="AT18" s="14">
+        <v>11391</v>
+      </c>
+      <c r="AU18" s="14">
+        <v>11748</v>
+      </c>
+      <c r="AV18" s="14">
+        <v>12343</v>
+      </c>
+      <c r="AW18" s="14">
+        <v>12329</v>
+      </c>
+      <c r="AX18" s="14">
+        <v>12451</v>
+      </c>
+      <c r="AY18" s="14">
+        <v>12658</v>
+      </c>
+      <c r="AZ18" s="14">
+        <v>13043</v>
+      </c>
+      <c r="BA18" s="14">
+        <v>13168</v>
+      </c>
+      <c r="BB18" s="14">
+        <v>13504</v>
+      </c>
+      <c r="BC18" s="14">
+        <v>15001</v>
+      </c>
+      <c r="BD18" s="14">
+        <v>16491</v>
+      </c>
+      <c r="BE18" s="14">
+        <v>18629</v>
+      </c>
+      <c r="BF18" s="14">
+        <v>19300</v>
+      </c>
+      <c r="BG18" s="13">
+        <v>18048</v>
+      </c>
+      <c r="BH18" s="10">
+        <v>16470</v>
+      </c>
+    </row>
+    <row r="20" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="AG20" s="16"/>
+      <c r="AH20" s="10"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:BD12">
-    <sortCondition ref="A3:A12"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB243748-DFB5-4F65-A856-C18F501810ED}">
-  <dimension ref="A1:B28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
-        <v>44029</v>
-      </c>
-      <c r="B2" s="14">
-        <v>8874</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>44036</v>
-      </c>
-      <c r="B3" s="14">
-        <v>9044</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>44043</v>
-      </c>
-      <c r="B4" s="14">
-        <v>8851</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>44050</v>
-      </c>
-      <c r="B5" s="14">
-        <v>9011</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>44057</v>
-      </c>
-      <c r="B6" s="14">
-        <v>10137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>44064</v>
-      </c>
-      <c r="B7" s="14">
-        <v>8829</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>44071</v>
-      </c>
-      <c r="B8" s="14">
-        <v>8652</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>44078</v>
-      </c>
-      <c r="B9" s="14">
-        <v>9048</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>44085</v>
-      </c>
-      <c r="B10" s="14">
-        <v>9135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>44092</v>
-      </c>
-      <c r="B11" s="14">
-        <v>9440</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>44099</v>
-      </c>
-      <c r="B12" s="14">
-        <v>9594</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>44106</v>
-      </c>
-      <c r="B13" s="14">
-        <v>9967</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>44113</v>
-      </c>
-      <c r="B14" s="14">
-        <v>10323</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <v>44120</v>
-      </c>
-      <c r="B15" s="14">
-        <v>10368</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
-        <v>44127</v>
-      </c>
-      <c r="B16" s="14">
-        <v>11062</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>44134</v>
-      </c>
-      <c r="B17" s="14">
-        <v>11393</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <v>44141</v>
-      </c>
-      <c r="B18" s="14">
-        <v>11755</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <v>44148</v>
-      </c>
-      <c r="B19" s="14">
-        <v>12348</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <v>44155</v>
-      </c>
-      <c r="B20" s="14">
-        <v>12313</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>44162</v>
-      </c>
-      <c r="B21" s="14">
-        <v>12443</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <v>44169</v>
-      </c>
-      <c r="B22" s="14">
-        <v>12656</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
-        <v>44176</v>
-      </c>
-      <c r="B23" s="14">
-        <v>13017</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
-        <v>44183</v>
-      </c>
-      <c r="B24" s="14">
-        <v>13140</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
-        <v>44190</v>
-      </c>
-      <c r="B25" s="14">
-        <v>13413</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
-        <v>44197</v>
-      </c>
-      <c r="B26" s="14">
-        <v>14747</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
-        <v>44204</v>
-      </c>
-      <c r="B27" s="14">
-        <v>16645</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
-        <v>44211</v>
-      </c>
-      <c r="B28" s="13">
-        <v>20004</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B27">
-    <sortCondition ref="A2:A27"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CEFF5B-2C83-4D1E-A565-E70539268DE8}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update evalulation of ONS estimates
</commit_message>
<xml_diff>
--- a/data/ons-deaths/explore/evaluation_of_ons_estimates.xlsx
+++ b/data/ons-deaths/explore/evaluation_of_ons_estimates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\covid-stats\data\ons-deaths\explore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB786113-A367-4DB0-9544-05A0B5AFDB03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EFB9EE-F973-430A-A268-B0AC161C5CE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{A515F7DA-6FDB-438E-B4AB-3C334154F930}"/>
   </bookViews>
@@ -1191,6 +1191,9 @@
                 <c:pt idx="15">
                   <c:v>44232</c:v>
                 </c:pt>
+                <c:pt idx="16">
+                  <c:v>44239</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1292,6 +1295,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>44232</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44239</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1400,6 +1406,9 @@
                 <c:pt idx="15">
                   <c:v>44232</c:v>
                 </c:pt>
+                <c:pt idx="16">
+                  <c:v>44239</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1508,6 +1517,9 @@
                 <c:pt idx="15">
                   <c:v>44232</c:v>
                 </c:pt>
+                <c:pt idx="16">
+                  <c:v>44239</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1619,6 +1631,9 @@
                 <c:pt idx="15">
                   <c:v>44232</c:v>
                 </c:pt>
+                <c:pt idx="16">
+                  <c:v>44239</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1733,6 +1748,9 @@
                 <c:pt idx="15">
                   <c:v>44232</c:v>
                 </c:pt>
+                <c:pt idx="16">
+                  <c:v>44239</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1849,6 +1867,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>44232</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44239</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1972,6 +1993,9 @@
                 <c:pt idx="15">
                   <c:v>44232</c:v>
                 </c:pt>
+                <c:pt idx="16">
+                  <c:v>44239</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2097,6 +2121,9 @@
                 <c:pt idx="15">
                   <c:v>44232</c:v>
                 </c:pt>
+                <c:pt idx="16">
+                  <c:v>44239</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2225,6 +2252,9 @@
                 <c:pt idx="15">
                   <c:v>44232</c:v>
                 </c:pt>
+                <c:pt idx="16">
+                  <c:v>44239</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2356,6 +2386,9 @@
                 <c:pt idx="15">
                   <c:v>44232</c:v>
                 </c:pt>
+                <c:pt idx="16">
+                  <c:v>44239</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2492,6 +2525,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>44232</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44239</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2818,6 +2854,102 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-C0CA-4F4D-8A7E-8BBD1C545922}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="15"/>
+          <c:order val="15"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6 </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AS$19:$ZZ$19</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="658"/>
+                <c:pt idx="0">
+                  <c:v>11039</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11393</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11764</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12345</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12320</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12455</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12658</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13045</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13167</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13515</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16523</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18692</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19455</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17977</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15955</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14064</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9531-4F65-BE85-EE335568B810}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3919,13 +4051,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D1BBA0-D981-49C0-9749-BCE3B566D49F}">
-  <dimension ref="A1:DF20"/>
+  <dimension ref="A1:DF48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="AS3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BK16" sqref="BK16"/>
+      <selection pane="bottomRight" activeCell="BG1" sqref="BG1:BI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4121,6 +4253,9 @@
       <c r="BH1" s="3">
         <v>5</v>
       </c>
+      <c r="BI1" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:110" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -4300,6 +4435,9 @@
       </c>
       <c r="BH2" s="6">
         <v>44232</v>
+      </c>
+      <c r="BI2" s="6">
+        <v>44239</v>
       </c>
     </row>
     <row r="3" spans="1:110" x14ac:dyDescent="0.25">
@@ -6386,7 +6524,7 @@
         <v>19288</v>
       </c>
     </row>
-    <row r="17" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>4</v>
       </c>
@@ -6474,7 +6612,7 @@
       </c>
       <c r="BH17" s="10"/>
     </row>
-    <row r="18" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>5</v>
       </c>
@@ -6562,11 +6700,235 @@
         <v>16470</v>
       </c>
     </row>
-    <row r="20" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="AG20" s="16"/>
-      <c r="AH20" s="10"/>
+    <row r="19" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>6</v>
+      </c>
+      <c r="AG19" s="16"/>
+      <c r="AH19" s="10"/>
+      <c r="AI19" s="14">
+        <v>10142</v>
+      </c>
+      <c r="AJ19" s="14">
+        <v>8836</v>
+      </c>
+      <c r="AK19" s="14">
+        <v>8657</v>
+      </c>
+      <c r="AL19" s="14">
+        <v>9046</v>
+      </c>
+      <c r="AM19" s="14">
+        <v>9142</v>
+      </c>
+      <c r="AN19" s="14">
+        <v>9467</v>
+      </c>
+      <c r="AO19" s="14">
+        <v>9595</v>
+      </c>
+      <c r="AP19" s="14">
+        <v>9968</v>
+      </c>
+      <c r="AQ19" s="14">
+        <v>10317</v>
+      </c>
+      <c r="AR19" s="14">
+        <v>10381</v>
+      </c>
+      <c r="AS19" s="14">
+        <v>11039</v>
+      </c>
+      <c r="AT19" s="14">
+        <v>11393</v>
+      </c>
+      <c r="AU19" s="14">
+        <v>11764</v>
+      </c>
+      <c r="AV19" s="14">
+        <v>12345</v>
+      </c>
+      <c r="AW19" s="14">
+        <v>12320</v>
+      </c>
+      <c r="AX19" s="14">
+        <v>12455</v>
+      </c>
+      <c r="AY19" s="14">
+        <v>12658</v>
+      </c>
+      <c r="AZ19" s="14">
+        <v>13045</v>
+      </c>
+      <c r="BA19" s="14">
+        <v>13167</v>
+      </c>
+      <c r="BB19" s="14">
+        <v>13515</v>
+      </c>
+      <c r="BC19" s="14">
+        <v>15014</v>
+      </c>
+      <c r="BD19" s="14">
+        <v>16523</v>
+      </c>
+      <c r="BE19" s="14">
+        <v>18692</v>
+      </c>
+      <c r="BF19" s="14">
+        <v>19455</v>
+      </c>
+      <c r="BG19" s="13">
+        <v>17977</v>
+      </c>
+      <c r="BH19" s="10">
+        <v>15955</v>
+      </c>
+      <c r="BI19" s="14">
+        <v>14064</v>
+      </c>
+    </row>
+    <row r="20" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AI20" s="14"/>
+      <c r="AJ20" s="14"/>
+      <c r="AK20" s="14"/>
+      <c r="AL20" s="14"/>
+      <c r="AM20" s="14"/>
+      <c r="AN20" s="14"/>
+      <c r="AO20" s="14"/>
+      <c r="AP20" s="14"/>
+      <c r="AQ20" s="14"/>
+      <c r="AR20" s="14"/>
+      <c r="AS20" s="14"/>
+      <c r="AT20" s="14"/>
+      <c r="AU20" s="14"/>
+      <c r="AV20" s="14"/>
+      <c r="AW20" s="14"/>
+      <c r="AX20" s="14"/>
+      <c r="AY20" s="14"/>
+      <c r="AZ20" s="14"/>
+      <c r="BA20" s="14"/>
+      <c r="BB20" s="14"/>
+      <c r="BC20" s="14"/>
+      <c r="BD20" s="14"/>
+      <c r="BE20" s="14"/>
+      <c r="BF20" s="14"/>
+      <c r="BG20" s="14"/>
+      <c r="BH20" s="14"/>
+      <c r="BI20" s="14"/>
+    </row>
+    <row r="22" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AI22" s="14"/>
+      <c r="AJ22" s="14"/>
+    </row>
+    <row r="23" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AI23" s="14"/>
+      <c r="AJ23" s="14"/>
+    </row>
+    <row r="24" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AI24" s="14"/>
+      <c r="AJ24" s="14"/>
+    </row>
+    <row r="25" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AI25" s="14"/>
+      <c r="AJ25" s="14"/>
+    </row>
+    <row r="26" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AI26" s="14"/>
+      <c r="AJ26" s="14"/>
+    </row>
+    <row r="27" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AI27" s="14"/>
+      <c r="AJ27" s="14"/>
+    </row>
+    <row r="28" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AI28" s="14"/>
+      <c r="AJ28" s="14"/>
+    </row>
+    <row r="29" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AI29" s="14"/>
+      <c r="AJ29" s="14"/>
+    </row>
+    <row r="30" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AI30" s="14"/>
+      <c r="AJ30" s="14"/>
+    </row>
+    <row r="31" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AI31" s="14"/>
+      <c r="AJ31" s="14"/>
+    </row>
+    <row r="32" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AI32" s="14"/>
+      <c r="AJ32" s="14"/>
+    </row>
+    <row r="33" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI33" s="14"/>
+      <c r="AJ33" s="14"/>
+    </row>
+    <row r="34" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI34" s="14"/>
+      <c r="AJ34" s="14"/>
+    </row>
+    <row r="35" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI35" s="14"/>
+      <c r="AJ35" s="14"/>
+    </row>
+    <row r="36" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI36" s="14"/>
+      <c r="AJ36" s="14"/>
+    </row>
+    <row r="37" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI37" s="14"/>
+      <c r="AJ37" s="14"/>
+    </row>
+    <row r="38" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI38" s="14"/>
+      <c r="AJ38" s="14"/>
+    </row>
+    <row r="39" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI39" s="14"/>
+      <c r="AJ39" s="14"/>
+    </row>
+    <row r="40" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI40" s="14"/>
+      <c r="AJ40" s="14"/>
+    </row>
+    <row r="41" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI41" s="14"/>
+      <c r="AJ41" s="14"/>
+    </row>
+    <row r="42" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI42" s="14"/>
+      <c r="AJ42" s="14"/>
+    </row>
+    <row r="43" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI43" s="14"/>
+      <c r="AJ43" s="14"/>
+    </row>
+    <row r="44" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI44" s="14"/>
+      <c r="AJ44" s="14"/>
+    </row>
+    <row r="45" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI45" s="14"/>
+      <c r="AJ45" s="14"/>
+    </row>
+    <row r="46" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI46" s="13"/>
+      <c r="AJ46" s="14"/>
+    </row>
+    <row r="47" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI47" s="10"/>
+      <c r="AJ47" s="14"/>
+    </row>
+    <row r="48" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI48" s="14"/>
+      <c r="AJ48" s="14"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AI22:AJ48">
+    <sortCondition descending="1" ref="AJ22:AJ48"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update evaluation of ONS estimates
</commit_message>
<xml_diff>
--- a/data/ons-deaths/explore/evaluation_of_ons_estimates.xlsx
+++ b/data/ons-deaths/explore/evaluation_of_ons_estimates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\covid-stats\data\ons-deaths\explore\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mike\projects\work\covid-stats\data\ons-deaths\explore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EFB9EE-F973-430A-A268-B0AC161C5CE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1A0C04-A715-408E-806E-40DA0440925F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{A515F7DA-6FDB-438E-B4AB-3C334154F930}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="General_)"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +135,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1194,6 +1200,12 @@
                 <c:pt idx="16">
                   <c:v>44239</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44253</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1298,6 +1310,12 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44239</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44253</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1409,6 +1427,12 @@
                 <c:pt idx="16">
                   <c:v>44239</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44253</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1520,6 +1544,12 @@
                 <c:pt idx="16">
                   <c:v>44239</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44253</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1634,6 +1664,12 @@
                 <c:pt idx="16">
                   <c:v>44239</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44253</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1751,6 +1787,12 @@
                 <c:pt idx="16">
                   <c:v>44239</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44253</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1870,6 +1912,12 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44239</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44253</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1996,6 +2044,12 @@
                 <c:pt idx="16">
                   <c:v>44239</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44253</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2124,6 +2178,12 @@
                 <c:pt idx="16">
                   <c:v>44239</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44253</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2255,6 +2315,12 @@
                 <c:pt idx="16">
                   <c:v>44239</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44253</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2389,6 +2455,12 @@
                 <c:pt idx="16">
                   <c:v>44239</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44253</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2528,6 +2600,12 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44239</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44253</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2950,6 +3028,207 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9531-4F65-BE85-EE335568B810}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="16"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7 </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AS$20:$ZZ$20</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="658"/>
+                <c:pt idx="0">
+                  <c:v>11033</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11393</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11769</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12340</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12328</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12450</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12659</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13051</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13153</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13527</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15017</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16523</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18701</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19472</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18112</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15831</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13824</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13272</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9951-4ECB-B739-A0828980D039}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="17"/>
+          <c:order val="17"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8 </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AS$21:$ZZ$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="658"/>
+                <c:pt idx="0">
+                  <c:v>11034</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11391</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11764</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12344</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12334</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12451</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12659</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13045</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13141</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13525</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15006</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16512</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18686</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19466</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18141</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15917</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13914</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13277</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11589</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9951-4ECB-B739-A0828980D039}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4051,13 +4330,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D1BBA0-D981-49C0-9749-BCE3B566D49F}">
-  <dimension ref="A1:DF48"/>
+  <dimension ref="A1:DF58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="AS3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BG1" sqref="BG1:BI2"/>
+      <selection pane="bottomRight" activeCell="Y39" sqref="Y39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4256,6 +4535,12 @@
       <c r="BI1" s="2">
         <v>6</v>
       </c>
+      <c r="BJ1" s="3">
+        <v>7</v>
+      </c>
+      <c r="BK1" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" spans="1:110" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -4438,6 +4723,12 @@
       </c>
       <c r="BI2" s="6">
         <v>44239</v>
+      </c>
+      <c r="BJ2" s="6">
+        <v>44246</v>
+      </c>
+      <c r="BK2" s="6">
+        <v>44253</v>
       </c>
     </row>
     <row r="3" spans="1:110" x14ac:dyDescent="0.25">
@@ -6524,7 +6815,7 @@
         <v>19288</v>
       </c>
     </row>
-    <row r="17" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>4</v>
       </c>
@@ -6612,7 +6903,7 @@
       </c>
       <c r="BH17" s="10"/>
     </row>
-    <row r="18" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>5</v>
       </c>
@@ -6700,7 +6991,7 @@
         <v>16470</v>
       </c>
     </row>
-    <row r="19" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>6</v>
       </c>
@@ -6788,147 +7079,573 @@
         <v>14064</v>
       </c>
     </row>
-    <row r="20" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>7</v>
+      </c>
       <c r="AI20" s="14"/>
-      <c r="AJ20" s="14"/>
-      <c r="AK20" s="14"/>
-      <c r="AL20" s="14"/>
-      <c r="AM20" s="14"/>
-      <c r="AN20" s="14"/>
-      <c r="AO20" s="14"/>
-      <c r="AP20" s="14"/>
-      <c r="AQ20" s="14"/>
-      <c r="AR20" s="14"/>
-      <c r="AS20" s="14"/>
-      <c r="AT20" s="14"/>
-      <c r="AU20" s="14"/>
-      <c r="AV20" s="14"/>
-      <c r="AW20" s="14"/>
-      <c r="AX20" s="14"/>
-      <c r="AY20" s="14"/>
-      <c r="AZ20" s="14"/>
-      <c r="BA20" s="14"/>
-      <c r="BB20" s="14"/>
-      <c r="BC20" s="14"/>
-      <c r="BD20" s="14"/>
-      <c r="BE20" s="14"/>
-      <c r="BF20" s="14"/>
-      <c r="BG20" s="14"/>
-      <c r="BH20" s="14"/>
-      <c r="BI20" s="14"/>
+      <c r="AJ20" s="10">
+        <v>8836</v>
+      </c>
+      <c r="AK20" s="10">
+        <v>8660</v>
+      </c>
+      <c r="AL20" s="10">
+        <v>9045</v>
+      </c>
+      <c r="AM20" s="10">
+        <v>9145</v>
+      </c>
+      <c r="AN20" s="10">
+        <v>9473</v>
+      </c>
+      <c r="AO20" s="10">
+        <v>9593</v>
+      </c>
+      <c r="AP20" s="10">
+        <v>9958</v>
+      </c>
+      <c r="AQ20" s="10">
+        <v>10316</v>
+      </c>
+      <c r="AR20" s="10">
+        <v>10383</v>
+      </c>
+      <c r="AS20" s="10">
+        <v>11033</v>
+      </c>
+      <c r="AT20" s="10">
+        <v>11393</v>
+      </c>
+      <c r="AU20" s="10">
+        <v>11769</v>
+      </c>
+      <c r="AV20" s="10">
+        <v>12340</v>
+      </c>
+      <c r="AW20" s="10">
+        <v>12328</v>
+      </c>
+      <c r="AX20" s="10">
+        <v>12450</v>
+      </c>
+      <c r="AY20" s="10">
+        <v>12659</v>
+      </c>
+      <c r="AZ20" s="10">
+        <v>13051</v>
+      </c>
+      <c r="BA20" s="10">
+        <v>13153</v>
+      </c>
+      <c r="BB20" s="10">
+        <v>13527</v>
+      </c>
+      <c r="BC20" s="10">
+        <v>15017</v>
+      </c>
+      <c r="BD20" s="10">
+        <v>16523</v>
+      </c>
+      <c r="BE20" s="10">
+        <v>18701</v>
+      </c>
+      <c r="BF20" s="10">
+        <v>19472</v>
+      </c>
+      <c r="BG20" s="10">
+        <v>18112</v>
+      </c>
+      <c r="BH20" s="10">
+        <v>15831</v>
+      </c>
+      <c r="BI20" s="10">
+        <v>13824</v>
+      </c>
+      <c r="BJ20" s="10">
+        <v>13272</v>
+      </c>
     </row>
-    <row r="22" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>8</v>
+      </c>
+      <c r="AK21" s="10">
+        <v>8655</v>
+      </c>
+      <c r="AL21" s="10">
+        <v>9039</v>
+      </c>
+      <c r="AM21" s="10">
+        <v>9144</v>
+      </c>
+      <c r="AN21" s="10">
+        <v>9475</v>
+      </c>
+      <c r="AO21" s="10">
+        <v>9591</v>
+      </c>
+      <c r="AP21" s="10">
+        <v>9948</v>
+      </c>
+      <c r="AQ21" s="10">
+        <v>10314</v>
+      </c>
+      <c r="AR21" s="10">
+        <v>10383</v>
+      </c>
+      <c r="AS21" s="10">
+        <v>11034</v>
+      </c>
+      <c r="AT21" s="10">
+        <v>11391</v>
+      </c>
+      <c r="AU21" s="10">
+        <v>11764</v>
+      </c>
+      <c r="AV21" s="10">
+        <v>12344</v>
+      </c>
+      <c r="AW21" s="10">
+        <v>12334</v>
+      </c>
+      <c r="AX21" s="10">
+        <v>12451</v>
+      </c>
+      <c r="AY21" s="10">
+        <v>12659</v>
+      </c>
+      <c r="AZ21" s="10">
+        <v>13045</v>
+      </c>
+      <c r="BA21" s="10">
+        <v>13141</v>
+      </c>
+      <c r="BB21" s="10">
+        <v>13525</v>
+      </c>
+      <c r="BC21" s="10">
+        <v>15006</v>
+      </c>
+      <c r="BD21" s="10">
+        <v>16512</v>
+      </c>
+      <c r="BE21" s="10">
+        <v>18686</v>
+      </c>
+      <c r="BF21" s="10">
+        <v>19466</v>
+      </c>
+      <c r="BG21" s="10">
+        <v>18141</v>
+      </c>
+      <c r="BH21" s="10">
+        <v>15917</v>
+      </c>
+      <c r="BI21" s="10">
+        <v>13914</v>
+      </c>
+      <c r="BJ21" s="10">
+        <v>13277</v>
+      </c>
+      <c r="BK21" s="10">
+        <v>11589</v>
+      </c>
+    </row>
+    <row r="22" spans="1:63" x14ac:dyDescent="0.25">
       <c r="AI22" s="14"/>
       <c r="AJ22" s="14"/>
     </row>
-    <row r="23" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:63" x14ac:dyDescent="0.25">
       <c r="AI23" s="14"/>
       <c r="AJ23" s="14"/>
     </row>
-    <row r="24" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:63" x14ac:dyDescent="0.25">
       <c r="AI24" s="14"/>
       <c r="AJ24" s="14"/>
     </row>
-    <row r="25" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:63" x14ac:dyDescent="0.25">
       <c r="AI25" s="14"/>
       <c r="AJ25" s="14"/>
     </row>
-    <row r="26" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:63" x14ac:dyDescent="0.25">
       <c r="AI26" s="14"/>
       <c r="AJ26" s="14"/>
     </row>
-    <row r="27" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:63" x14ac:dyDescent="0.25">
       <c r="AI27" s="14"/>
       <c r="AJ27" s="14"/>
     </row>
-    <row r="28" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:63" x14ac:dyDescent="0.25">
       <c r="AI28" s="14"/>
       <c r="AJ28" s="14"/>
     </row>
-    <row r="29" spans="1:61" x14ac:dyDescent="0.25">
-      <c r="AI29" s="14"/>
-      <c r="AJ29" s="14"/>
+    <row r="29" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="W29">
+        <v>11589</v>
+      </c>
+      <c r="X29">
+        <v>13277</v>
+      </c>
+      <c r="Y29">
+        <v>13914</v>
+      </c>
+      <c r="Z29">
+        <v>15917</v>
+      </c>
+      <c r="AA29">
+        <v>18141</v>
+      </c>
+      <c r="AB29">
+        <v>19466</v>
+      </c>
+      <c r="AC29">
+        <v>18686</v>
+      </c>
+      <c r="AD29">
+        <v>16512</v>
+      </c>
+      <c r="AE29">
+        <v>15006</v>
+      </c>
+      <c r="AF29">
+        <v>13525</v>
+      </c>
+      <c r="AG29">
+        <v>13141</v>
+      </c>
+      <c r="AH29">
+        <v>13045</v>
+      </c>
+      <c r="AI29" s="14">
+        <v>12659</v>
+      </c>
+      <c r="AJ29" s="14">
+        <v>12451</v>
+      </c>
+      <c r="AK29">
+        <v>12334</v>
+      </c>
+      <c r="AL29">
+        <v>12344</v>
+      </c>
+      <c r="AM29">
+        <v>11764</v>
+      </c>
+      <c r="AN29">
+        <v>11391</v>
+      </c>
+      <c r="AO29">
+        <v>11034</v>
+      </c>
+      <c r="AP29">
+        <v>10383</v>
+      </c>
+      <c r="AQ29">
+        <v>10314</v>
+      </c>
+      <c r="AR29">
+        <v>9948</v>
+      </c>
+      <c r="AS29">
+        <v>9591</v>
+      </c>
+      <c r="AT29">
+        <v>9475</v>
+      </c>
+      <c r="AU29">
+        <v>9144</v>
+      </c>
+      <c r="AV29">
+        <v>9039</v>
+      </c>
+      <c r="AW29">
+        <v>8655</v>
+      </c>
     </row>
-    <row r="30" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:63" x14ac:dyDescent="0.25">
       <c r="AI30" s="14"/>
       <c r="AJ30" s="14"/>
     </row>
-    <row r="31" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="Y31">
+        <v>8655</v>
+      </c>
+      <c r="Z31">
+        <v>1</v>
+      </c>
       <c r="AI31" s="14"/>
       <c r="AJ31" s="14"/>
     </row>
-    <row r="32" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="Y32">
+        <v>9039</v>
+      </c>
+      <c r="Z32">
+        <v>2</v>
+      </c>
       <c r="AI32" s="14"/>
       <c r="AJ32" s="14"/>
     </row>
-    <row r="33" spans="35:36" x14ac:dyDescent="0.25">
+    <row r="33" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y33">
+        <v>9144</v>
+      </c>
+      <c r="Z33">
+        <v>3</v>
+      </c>
       <c r="AI33" s="14"/>
       <c r="AJ33" s="14"/>
     </row>
-    <row r="34" spans="35:36" x14ac:dyDescent="0.25">
+    <row r="34" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y34">
+        <v>9475</v>
+      </c>
+      <c r="Z34">
+        <v>4</v>
+      </c>
       <c r="AI34" s="14"/>
       <c r="AJ34" s="14"/>
     </row>
-    <row r="35" spans="35:36" x14ac:dyDescent="0.25">
+    <row r="35" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y35">
+        <v>9591</v>
+      </c>
+      <c r="Z35">
+        <v>5</v>
+      </c>
       <c r="AI35" s="14"/>
       <c r="AJ35" s="14"/>
     </row>
-    <row r="36" spans="35:36" x14ac:dyDescent="0.25">
+    <row r="36" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y36">
+        <v>9948</v>
+      </c>
+      <c r="Z36">
+        <v>6</v>
+      </c>
       <c r="AI36" s="14"/>
       <c r="AJ36" s="14"/>
     </row>
-    <row r="37" spans="35:36" x14ac:dyDescent="0.25">
+    <row r="37" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y37">
+        <v>10314</v>
+      </c>
+      <c r="Z37">
+        <v>7</v>
+      </c>
       <c r="AI37" s="14"/>
       <c r="AJ37" s="14"/>
     </row>
-    <row r="38" spans="35:36" x14ac:dyDescent="0.25">
+    <row r="38" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y38">
+        <v>10383</v>
+      </c>
+      <c r="Z38">
+        <v>8</v>
+      </c>
       <c r="AI38" s="14"/>
       <c r="AJ38" s="14"/>
     </row>
-    <row r="39" spans="35:36" x14ac:dyDescent="0.25">
+    <row r="39" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y39">
+        <v>11034</v>
+      </c>
+      <c r="Z39">
+        <v>9</v>
+      </c>
       <c r="AI39" s="14"/>
       <c r="AJ39" s="14"/>
     </row>
-    <row r="40" spans="35:36" x14ac:dyDescent="0.25">
+    <row r="40" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y40">
+        <v>11391</v>
+      </c>
+      <c r="Z40">
+        <v>10</v>
+      </c>
       <c r="AI40" s="14"/>
       <c r="AJ40" s="14"/>
     </row>
-    <row r="41" spans="35:36" x14ac:dyDescent="0.25">
+    <row r="41" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y41">
+        <v>11764</v>
+      </c>
+      <c r="Z41">
+        <v>11</v>
+      </c>
       <c r="AI41" s="14"/>
       <c r="AJ41" s="14"/>
     </row>
-    <row r="42" spans="35:36" x14ac:dyDescent="0.25">
+    <row r="42" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y42">
+        <v>12344</v>
+      </c>
+      <c r="Z42">
+        <v>12</v>
+      </c>
       <c r="AI42" s="14"/>
       <c r="AJ42" s="14"/>
     </row>
-    <row r="43" spans="35:36" x14ac:dyDescent="0.25">
+    <row r="43" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y43">
+        <v>12334</v>
+      </c>
+      <c r="Z43">
+        <v>13</v>
+      </c>
       <c r="AI43" s="14"/>
       <c r="AJ43" s="14"/>
     </row>
-    <row r="44" spans="35:36" x14ac:dyDescent="0.25">
+    <row r="44" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y44">
+        <v>12451</v>
+      </c>
+      <c r="Z44">
+        <v>14</v>
+      </c>
       <c r="AI44" s="14"/>
       <c r="AJ44" s="14"/>
     </row>
-    <row r="45" spans="35:36" x14ac:dyDescent="0.25">
+    <row r="45" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y45">
+        <v>12659</v>
+      </c>
+      <c r="Z45">
+        <v>15</v>
+      </c>
       <c r="AI45" s="14"/>
       <c r="AJ45" s="14"/>
     </row>
-    <row r="46" spans="35:36" x14ac:dyDescent="0.25">
-      <c r="AI46" s="13"/>
+    <row r="46" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y46">
+        <v>13045</v>
+      </c>
+      <c r="Z46">
+        <v>16</v>
+      </c>
+      <c r="AI46" s="14"/>
       <c r="AJ46" s="14"/>
     </row>
-    <row r="47" spans="35:36" x14ac:dyDescent="0.25">
-      <c r="AI47" s="10"/>
+    <row r="47" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y47">
+        <v>13141</v>
+      </c>
+      <c r="Z47">
+        <v>17</v>
+      </c>
+      <c r="AI47" s="14"/>
       <c r="AJ47" s="14"/>
     </row>
-    <row r="48" spans="35:36" x14ac:dyDescent="0.25">
+    <row r="48" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y48">
+        <v>13525</v>
+      </c>
+      <c r="Z48">
+        <v>18</v>
+      </c>
       <c r="AI48" s="14"/>
       <c r="AJ48" s="14"/>
     </row>
+    <row r="49" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y49">
+        <v>15006</v>
+      </c>
+      <c r="Z49">
+        <v>19</v>
+      </c>
+      <c r="AI49" s="14"/>
+      <c r="AJ49" s="14"/>
+    </row>
+    <row r="50" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y50">
+        <v>16512</v>
+      </c>
+      <c r="Z50">
+        <v>20</v>
+      </c>
+      <c r="AI50" s="14"/>
+      <c r="AJ50" s="14"/>
+    </row>
+    <row r="51" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y51">
+        <v>18686</v>
+      </c>
+      <c r="Z51">
+        <v>21</v>
+      </c>
+      <c r="AI51" s="14"/>
+      <c r="AJ51" s="14"/>
+    </row>
+    <row r="52" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y52">
+        <v>19466</v>
+      </c>
+      <c r="Z52">
+        <v>22</v>
+      </c>
+      <c r="AI52" s="14"/>
+      <c r="AJ52" s="14"/>
+    </row>
+    <row r="53" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y53">
+        <v>18141</v>
+      </c>
+      <c r="Z53">
+        <v>23</v>
+      </c>
+      <c r="AI53" s="14"/>
+      <c r="AJ53" s="14"/>
+    </row>
+    <row r="54" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y54">
+        <v>15917</v>
+      </c>
+      <c r="Z54">
+        <v>24</v>
+      </c>
+      <c r="AI54" s="14"/>
+      <c r="AJ54" s="14"/>
+    </row>
+    <row r="55" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y55">
+        <v>13914</v>
+      </c>
+      <c r="Z55">
+        <v>25</v>
+      </c>
+      <c r="AI55" s="14"/>
+      <c r="AJ55" s="14"/>
+    </row>
+    <row r="56" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y56">
+        <v>13277</v>
+      </c>
+      <c r="Z56">
+        <v>26</v>
+      </c>
+      <c r="AI56" s="14"/>
+      <c r="AJ56" s="14"/>
+    </row>
+    <row r="57" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y57">
+        <v>11589</v>
+      </c>
+      <c r="Z57">
+        <v>27</v>
+      </c>
+      <c r="AI57" s="14"/>
+      <c r="AJ57" s="14"/>
+    </row>
+    <row r="58" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="AI58" s="14"/>
+      <c r="AJ58" s="14"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AI22:AJ48">
-    <sortCondition descending="1" ref="AJ22:AJ48"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Y31:Z57">
+    <sortCondition ref="Z31:Z57"/>
   </sortState>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6938,7 +7655,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Seed ONS weekly estimates
</commit_message>
<xml_diff>
--- a/data/ons-deaths/explore/evaluation_of_ons_estimates.xlsx
+++ b/data/ons-deaths/explore/evaluation_of_ons_estimates.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mike\projects\work\covid-stats\data\ons-deaths\explore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4F8923-5CB8-49D1-89A6-821CF0418B0A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18ED4A52-E011-4904-844A-D70DCB91157B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{A515F7DA-6FDB-438E-B4AB-3C334154F930}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="chart" sheetId="3" r:id="rId2"/>
+    <sheet name="seed" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,21 +27,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Week number</t>
   </si>
   <si>
     <t>Week ended</t>
   </si>
+  <si>
+    <t>estimated_occurrences</t>
+  </si>
+  <si>
+    <t>week_ended</t>
+  </si>
+  <si>
+    <t>week_number</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="General_)"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -604,7 +615,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -646,6 +657,7 @@
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="380">
     <cellStyle name="Comma 10" xfId="207" xr:uid="{68760587-A681-4C1F-B0D4-59CF710E7957}"/>
@@ -4473,10 +4485,10 @@
   <dimension ref="A1:DF58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AS19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="BL22" sqref="A1:BL22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7972,4 +7984,721 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C97F18-DB2D-4BF4-AF5D-B410B710A6FA}">
+  <dimension ref="A1:C63"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B63" sqref="B63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="17">
+        <v>43833</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>12431</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
+        <v>43840</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>12139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>43847</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>11746</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>43854</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>10914</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>43861</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>11094</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <v>43868</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>10710</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
+        <v>43875</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>10877</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
+        <v>43882</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>10795</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
+        <v>43889</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>10647</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
+        <v>43896</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>10984</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
+        <v>43903</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>10834</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
+        <v>43910</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>11401</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
+        <v>43917</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>13787</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="17">
+        <v>43924</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>17897</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="17">
+        <v>43931</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>22038</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="17">
+        <v>43938</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>20922</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
+        <v>43945</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>18694</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>43952</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>15825</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
+        <v>43959</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>13712</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
+        <v>43966</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>11948</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="17">
+        <v>43973</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>11354</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="17">
+        <v>43980</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>10216</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="17">
+        <v>43987</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>9971</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="17">
+        <v>43994</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>9453</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="17">
+        <v>44001</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>9204</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="17">
+        <v>44008</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>9661</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="17">
+        <v>44015</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>8740</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="17">
+        <v>44022</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>8662</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="17">
+        <v>44029</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>8874</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="17">
+        <v>44036</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>9050</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="17">
+        <v>44043</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>8852</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="17">
+        <v>44050</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>9008</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="17">
+        <v>44057</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>10142</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="17">
+        <v>44064</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>8836</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="17">
+        <v>44071</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>8655</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="17">
+        <v>44078</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>9033</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="17">
+        <v>44085</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <v>9143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="17">
+        <v>44092</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <v>9474</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="17">
+        <v>44099</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <v>9584</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="17">
+        <v>44106</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>9957</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="17">
+        <v>44113</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <v>10308</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="17">
+        <v>44120</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <v>10384</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="17">
+        <v>44127</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <v>11031</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="17">
+        <v>44134</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <v>11388</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="17">
+        <v>44141</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <v>11754</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="17">
+        <v>44148</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <v>12339</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="17">
+        <v>44155</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <v>12326</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="17">
+        <v>44162</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <v>12447</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="17">
+        <v>44169</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>12675</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="17">
+        <v>44176</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <v>13045</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="17">
+        <v>44183</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52">
+        <v>13138</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="17">
+        <v>44190</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53">
+        <v>13532</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="17">
+        <v>44197</v>
+      </c>
+      <c r="B54">
+        <v>53</v>
+      </c>
+      <c r="C54">
+        <v>15012</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="17">
+        <v>44204</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>16507</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="17">
+        <v>44211</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56">
+        <v>18696</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="17">
+        <v>44218</v>
+      </c>
+      <c r="B57">
+        <v>3</v>
+      </c>
+      <c r="C57">
+        <v>19473</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="17">
+        <v>44225</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58">
+        <v>18160</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="17">
+        <v>44232</v>
+      </c>
+      <c r="B59">
+        <v>5</v>
+      </c>
+      <c r="C59">
+        <v>15920</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="17">
+        <v>44239</v>
+      </c>
+      <c r="B60">
+        <v>6</v>
+      </c>
+      <c r="C60">
+        <v>13983</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="17">
+        <v>44246</v>
+      </c>
+      <c r="B61">
+        <v>7</v>
+      </c>
+      <c r="C61">
+        <v>13281</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="17">
+        <v>44253</v>
+      </c>
+      <c r="B62">
+        <v>8</v>
+      </c>
+      <c r="C62">
+        <v>11745</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="17">
+        <v>44260</v>
+      </c>
+      <c r="B63">
+        <v>9</v>
+      </c>
+      <c r="C63">
+        <v>10480</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update review of ONS estimates
</commit_message>
<xml_diff>
--- a/data/ons-deaths/explore/evaluation_of_ons_estimates.xlsx
+++ b/data/ons-deaths/explore/evaluation_of_ons_estimates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mike\projects\work\covid-stats\data\ons-deaths\explore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18ED4A52-E011-4904-844A-D70DCB91157B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBA8442-8351-4673-BE8B-C9AF0124DE94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{A515F7DA-6FDB-438E-B4AB-3C334154F930}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <numFmt numFmtId="164" formatCode="General_)"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +153,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -615,7 +621,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -658,6 +664,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="380">
     <cellStyle name="Comma 10" xfId="207" xr:uid="{68760587-A681-4C1F-B0D4-59CF710E7957}"/>
@@ -1221,6 +1230,9 @@
                 <c:pt idx="19">
                   <c:v>44260</c:v>
                 </c:pt>
+                <c:pt idx="20">
+                  <c:v>44267</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1334,6 +1346,9 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>44260</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44267</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1454,6 +1469,9 @@
                 <c:pt idx="19">
                   <c:v>44260</c:v>
                 </c:pt>
+                <c:pt idx="20">
+                  <c:v>44267</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1574,6 +1592,9 @@
                 <c:pt idx="19">
                   <c:v>44260</c:v>
                 </c:pt>
+                <c:pt idx="20">
+                  <c:v>44267</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1697,6 +1718,9 @@
                 <c:pt idx="19">
                   <c:v>44260</c:v>
                 </c:pt>
+                <c:pt idx="20">
+                  <c:v>44267</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1823,6 +1847,9 @@
                 <c:pt idx="19">
                   <c:v>44260</c:v>
                 </c:pt>
+                <c:pt idx="20">
+                  <c:v>44267</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1951,6 +1978,9 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>44260</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44267</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2086,6 +2116,9 @@
                 <c:pt idx="19">
                   <c:v>44260</c:v>
                 </c:pt>
+                <c:pt idx="20">
+                  <c:v>44267</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2223,6 +2256,9 @@
                 <c:pt idx="19">
                   <c:v>44260</c:v>
                 </c:pt>
+                <c:pt idx="20">
+                  <c:v>44267</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2363,6 +2399,9 @@
                 <c:pt idx="19">
                   <c:v>44260</c:v>
                 </c:pt>
+                <c:pt idx="20">
+                  <c:v>44267</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2506,6 +2545,9 @@
                 <c:pt idx="19">
                   <c:v>44260</c:v>
                 </c:pt>
+                <c:pt idx="20">
+                  <c:v>44267</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2654,6 +2696,9 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>44260</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44267</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3381,6 +3426,113 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-BC5E-4175-BA99-51106D73A680}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="19"/>
+          <c:order val="19"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10 </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AS$23:$ZZ$23</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="658"/>
+                <c:pt idx="0">
+                  <c:v>11029</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11388</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11757</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12326</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12325</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12442</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12665</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13056</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13137</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13532</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15011</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16510</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18682</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19479</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18155</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15936</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13342</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11717</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10438</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10657</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4F88-4997-8C48-765558F1826F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4482,13 +4634,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D1BBA0-D981-49C0-9749-BCE3B566D49F}">
-  <dimension ref="A1:DF58"/>
+  <dimension ref="A1:DF59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="AS18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BL22" sqref="A1:BL22"/>
+      <selection pane="bottomRight" activeCell="BK1" sqref="BK1:BM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4696,6 +4848,9 @@
       <c r="BL1" s="3">
         <v>9</v>
       </c>
+      <c r="BM1" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" spans="1:110" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -4887,6 +5042,9 @@
       </c>
       <c r="BL2" s="6">
         <v>44260</v>
+      </c>
+      <c r="BM2" s="6">
+        <v>44267</v>
       </c>
     </row>
     <row r="3" spans="1:110" x14ac:dyDescent="0.25">
@@ -6973,7 +7131,7 @@
         <v>19288</v>
       </c>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>4</v>
       </c>
@@ -7061,7 +7219,7 @@
       </c>
       <c r="BH17" s="10"/>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>5</v>
       </c>
@@ -7149,7 +7307,7 @@
         <v>16470</v>
       </c>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>6</v>
       </c>
@@ -7237,7 +7395,7 @@
         <v>14064</v>
       </c>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>7</v>
       </c>
@@ -7324,7 +7482,7 @@
         <v>13272</v>
       </c>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>8</v>
       </c>
@@ -7410,7 +7568,7 @@
         <v>11589</v>
       </c>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>9</v>
       </c>
@@ -7498,473 +7656,425 @@
         <v>10480</v>
       </c>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>10</v>
+      </c>
       <c r="AI23" s="14"/>
       <c r="AJ23" s="14"/>
-    </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="AL23" s="10"/>
+      <c r="AM23" s="18">
+        <v>9140</v>
+      </c>
+      <c r="AN23" s="18">
+        <v>9474</v>
+      </c>
+      <c r="AO23" s="18">
+        <v>9591</v>
+      </c>
+      <c r="AP23" s="18">
+        <v>9960</v>
+      </c>
+      <c r="AQ23" s="18">
+        <v>10306</v>
+      </c>
+      <c r="AR23" s="18">
+        <v>10376</v>
+      </c>
+      <c r="AS23" s="18">
+        <v>11029</v>
+      </c>
+      <c r="AT23" s="18">
+        <v>11388</v>
+      </c>
+      <c r="AU23" s="18">
+        <v>11757</v>
+      </c>
+      <c r="AV23" s="18">
+        <v>12326</v>
+      </c>
+      <c r="AW23" s="18">
+        <v>12325</v>
+      </c>
+      <c r="AX23" s="18">
+        <v>12442</v>
+      </c>
+      <c r="AY23" s="18">
+        <v>12665</v>
+      </c>
+      <c r="AZ23" s="18">
+        <v>13056</v>
+      </c>
+      <c r="BA23" s="18">
+        <v>13137</v>
+      </c>
+      <c r="BB23" s="18">
+        <v>13532</v>
+      </c>
+      <c r="BC23" s="18">
+        <v>15011</v>
+      </c>
+      <c r="BD23" s="18">
+        <v>16510</v>
+      </c>
+      <c r="BE23" s="18">
+        <v>18682</v>
+      </c>
+      <c r="BF23" s="18">
+        <v>19479</v>
+      </c>
+      <c r="BG23" s="18">
+        <v>18155</v>
+      </c>
+      <c r="BH23" s="18">
+        <v>15936</v>
+      </c>
+      <c r="BI23" s="18">
+        <v>14001</v>
+      </c>
+      <c r="BJ23" s="18">
+        <v>13342</v>
+      </c>
+      <c r="BK23" s="18">
+        <v>11717</v>
+      </c>
+      <c r="BL23" s="18">
+        <v>10438</v>
+      </c>
+      <c r="BM23" s="18">
+        <v>10657</v>
+      </c>
+    </row>
+    <row r="24" spans="1:65" x14ac:dyDescent="0.25">
       <c r="AI24" s="14"/>
       <c r="AJ24" s="14"/>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:65" x14ac:dyDescent="0.25">
       <c r="AI25" s="14"/>
       <c r="AJ25" s="14"/>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:65" x14ac:dyDescent="0.25">
       <c r="AI26" s="14"/>
       <c r="AJ26" s="14"/>
     </row>
-    <row r="27" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:65" x14ac:dyDescent="0.25">
       <c r="AI27" s="14"/>
       <c r="AJ27" s="14"/>
     </row>
-    <row r="28" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="W28">
-        <v>27</v>
-      </c>
-      <c r="X28">
-        <v>26</v>
-      </c>
-      <c r="Y28">
-        <v>25</v>
-      </c>
-      <c r="Z28">
-        <v>24</v>
-      </c>
-      <c r="AA28">
-        <v>23</v>
-      </c>
-      <c r="AB28">
-        <v>22</v>
-      </c>
-      <c r="AC28">
-        <v>21</v>
-      </c>
-      <c r="AD28">
-        <v>20</v>
-      </c>
-      <c r="AE28">
-        <v>19</v>
-      </c>
-      <c r="AF28">
-        <v>18</v>
-      </c>
-      <c r="AG28">
-        <v>17</v>
-      </c>
-      <c r="AH28">
-        <v>16</v>
-      </c>
-      <c r="AI28">
-        <v>15</v>
-      </c>
-      <c r="AJ28">
-        <v>14</v>
-      </c>
-      <c r="AK28">
-        <v>13</v>
-      </c>
-      <c r="AL28">
-        <v>12</v>
-      </c>
-      <c r="AM28">
-        <v>11</v>
-      </c>
-      <c r="AN28">
-        <v>10</v>
-      </c>
-      <c r="AO28">
-        <v>9</v>
-      </c>
-      <c r="AP28">
-        <v>8</v>
-      </c>
-      <c r="AQ28">
-        <v>7</v>
-      </c>
-      <c r="AR28">
-        <v>6</v>
-      </c>
-      <c r="AS28">
-        <v>5</v>
-      </c>
-      <c r="AT28">
-        <v>4</v>
-      </c>
-      <c r="AU28">
-        <v>3</v>
-      </c>
-      <c r="AV28">
-        <v>2</v>
-      </c>
-      <c r="AW28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="W29" s="10">
-        <v>10480</v>
-      </c>
-      <c r="X29" s="10">
-        <v>11745</v>
-      </c>
-      <c r="Y29" s="10">
-        <v>13281</v>
-      </c>
-      <c r="Z29" s="10">
-        <v>13983</v>
-      </c>
-      <c r="AA29" s="10">
-        <v>15920</v>
-      </c>
-      <c r="AB29" s="10">
-        <v>18160</v>
-      </c>
-      <c r="AC29" s="10">
-        <v>19473</v>
-      </c>
-      <c r="AD29" s="10">
-        <v>18696</v>
-      </c>
-      <c r="AE29" s="10">
-        <v>16507</v>
-      </c>
-      <c r="AF29" s="10">
-        <v>15012</v>
-      </c>
-      <c r="AG29" s="10">
-        <v>13532</v>
-      </c>
-      <c r="AH29" s="10">
-        <v>13138</v>
-      </c>
-      <c r="AI29" s="10">
-        <v>13045</v>
-      </c>
-      <c r="AJ29" s="10">
-        <v>12675</v>
-      </c>
-      <c r="AK29" s="10">
-        <v>12447</v>
-      </c>
-      <c r="AL29" s="10">
-        <v>12326</v>
-      </c>
-      <c r="AM29" s="10">
-        <v>12339</v>
-      </c>
-      <c r="AN29" s="10">
-        <v>11754</v>
-      </c>
-      <c r="AO29" s="10">
-        <v>11388</v>
-      </c>
-      <c r="AP29" s="10">
-        <v>11031</v>
-      </c>
-      <c r="AQ29" s="10">
-        <v>10384</v>
-      </c>
-      <c r="AR29" s="10">
-        <v>10308</v>
-      </c>
-      <c r="AS29" s="10">
-        <v>9957</v>
-      </c>
-      <c r="AT29" s="10">
-        <v>9584</v>
-      </c>
-      <c r="AU29" s="10">
-        <v>9474</v>
-      </c>
-      <c r="AV29" s="10">
-        <v>9143</v>
-      </c>
-      <c r="AW29" s="10">
-        <v>9033</v>
-      </c>
-    </row>
-    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="AI30" s="14"/>
-      <c r="AJ30" s="14"/>
-    </row>
-    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="Y31" s="10">
-        <v>9033</v>
-      </c>
-      <c r="Z31">
-        <v>27</v>
-      </c>
+    <row r="28" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="AI28" s="14"/>
+      <c r="AJ28" s="14"/>
+    </row>
+    <row r="30" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="W30" s="10"/>
+      <c r="X30" s="10"/>
+      <c r="Y30" s="10"/>
+      <c r="Z30" s="10"/>
+      <c r="AA30" s="10"/>
+      <c r="AB30" s="10"/>
+      <c r="AC30" s="10"/>
+      <c r="AD30" s="10"/>
+      <c r="AE30" s="10"/>
+      <c r="AF30" s="10"/>
+      <c r="AG30" s="10"/>
+      <c r="AH30" s="10"/>
+      <c r="AI30" s="10"/>
+      <c r="AJ30" s="10"/>
+      <c r="AK30" s="10"/>
+      <c r="AL30" s="10"/>
+      <c r="AM30" s="10"/>
+      <c r="AN30" s="10"/>
+      <c r="AO30" s="10"/>
+      <c r="AP30" s="10"/>
+      <c r="AQ30" s="10"/>
+      <c r="AR30" s="10"/>
+      <c r="AS30" s="10"/>
+      <c r="AT30" s="10"/>
+      <c r="AU30" s="10"/>
+      <c r="AV30" s="10"/>
+      <c r="AW30" s="10"/>
+    </row>
+    <row r="31" spans="1:65" x14ac:dyDescent="0.25">
       <c r="AI31" s="14"/>
       <c r="AJ31" s="14"/>
     </row>
-    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="Y32" s="10">
-        <v>9143</v>
+    <row r="32" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="Y32" s="18">
+        <v>9140</v>
       </c>
       <c r="Z32">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="AI32" s="14"/>
       <c r="AJ32" s="14"/>
     </row>
     <row r="33" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y33" s="10">
+      <c r="Y33" s="18">
         <v>9474</v>
       </c>
       <c r="Z33">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="AI33" s="14"/>
       <c r="AJ33" s="14"/>
     </row>
     <row r="34" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y34" s="10">
-        <v>9584</v>
+      <c r="Y34" s="18">
+        <v>9591</v>
       </c>
       <c r="Z34">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="AI34" s="14"/>
       <c r="AJ34" s="14"/>
     </row>
     <row r="35" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y35" s="10">
-        <v>9957</v>
+      <c r="Y35" s="18">
+        <v>9960</v>
       </c>
       <c r="Z35">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="AI35" s="14"/>
       <c r="AJ35" s="14"/>
     </row>
     <row r="36" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y36" s="10">
-        <v>10308</v>
+      <c r="Y36" s="18">
+        <v>10306</v>
       </c>
       <c r="Z36">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="AI36" s="14"/>
       <c r="AJ36" s="14"/>
     </row>
     <row r="37" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y37" s="10">
-        <v>10384</v>
+      <c r="Y37" s="18">
+        <v>10376</v>
       </c>
       <c r="Z37">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="AI37" s="14"/>
       <c r="AJ37" s="14"/>
     </row>
     <row r="38" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y38" s="10">
-        <v>11031</v>
+      <c r="Y38" s="18">
+        <v>11029</v>
       </c>
       <c r="Z38">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="AI38" s="14"/>
       <c r="AJ38" s="14"/>
     </row>
     <row r="39" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y39" s="10">
+      <c r="Y39" s="18">
         <v>11388</v>
       </c>
       <c r="Z39">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="AI39" s="14"/>
       <c r="AJ39" s="14"/>
     </row>
     <row r="40" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y40" s="10">
-        <v>11754</v>
+      <c r="Y40" s="18">
+        <v>11757</v>
       </c>
       <c r="Z40">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="AI40" s="14"/>
       <c r="AJ40" s="14"/>
     </row>
     <row r="41" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y41" s="10">
-        <v>12339</v>
+      <c r="Y41" s="18">
+        <v>12326</v>
       </c>
       <c r="Z41">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="AI41" s="14"/>
       <c r="AJ41" s="14"/>
     </row>
     <row r="42" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y42" s="10">
-        <v>12326</v>
+      <c r="Y42" s="18">
+        <v>12325</v>
       </c>
       <c r="Z42">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="AI42" s="14"/>
       <c r="AJ42" s="14"/>
     </row>
     <row r="43" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y43" s="10">
-        <v>12447</v>
+      <c r="Y43" s="18">
+        <v>12442</v>
       </c>
       <c r="Z43">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AI43" s="14"/>
       <c r="AJ43" s="14"/>
     </row>
     <row r="44" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y44" s="10">
-        <v>12675</v>
+      <c r="Y44" s="18">
+        <v>12665</v>
       </c>
       <c r="Z44">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AI44" s="14"/>
       <c r="AJ44" s="14"/>
     </row>
     <row r="45" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y45" s="10">
-        <v>13045</v>
+      <c r="Y45" s="18">
+        <v>13056</v>
       </c>
       <c r="Z45">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AI45" s="14"/>
       <c r="AJ45" s="14"/>
     </row>
     <row r="46" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y46" s="10">
-        <v>13138</v>
+      <c r="Y46" s="18">
+        <v>13137</v>
       </c>
       <c r="Z46">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AI46" s="14"/>
       <c r="AJ46" s="14"/>
     </row>
     <row r="47" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y47" s="10">
+      <c r="Y47" s="18">
         <v>13532</v>
       </c>
       <c r="Z47">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="AI47" s="14"/>
       <c r="AJ47" s="14"/>
     </row>
     <row r="48" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y48" s="10">
-        <v>15012</v>
+      <c r="Y48" s="18">
+        <v>15011</v>
       </c>
       <c r="Z48">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="AI48" s="14"/>
       <c r="AJ48" s="14"/>
     </row>
     <row r="49" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y49" s="10">
-        <v>16507</v>
+      <c r="Y49" s="18">
+        <v>16510</v>
       </c>
       <c r="Z49">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="AI49" s="14"/>
       <c r="AJ49" s="14"/>
     </row>
     <row r="50" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y50" s="10">
-        <v>18696</v>
+      <c r="Y50" s="18">
+        <v>18682</v>
       </c>
       <c r="Z50">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="AI50" s="14"/>
       <c r="AJ50" s="14"/>
     </row>
     <row r="51" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y51" s="10">
-        <v>19473</v>
+      <c r="Y51" s="18">
+        <v>19479</v>
       </c>
       <c r="Z51">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="AI51" s="14"/>
       <c r="AJ51" s="14"/>
     </row>
     <row r="52" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y52" s="10">
-        <v>18160</v>
+      <c r="Y52" s="18">
+        <v>18155</v>
       </c>
       <c r="Z52">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="AI52" s="14"/>
       <c r="AJ52" s="14"/>
     </row>
     <row r="53" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y53" s="10">
-        <v>15920</v>
+      <c r="Y53" s="18">
+        <v>15936</v>
       </c>
       <c r="Z53">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="AI53" s="14"/>
       <c r="AJ53" s="14"/>
     </row>
     <row r="54" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y54" s="10">
-        <v>13983</v>
+      <c r="Y54" s="18">
+        <v>14001</v>
       </c>
       <c r="Z54">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="AI54" s="14"/>
       <c r="AJ54" s="14"/>
     </row>
     <row r="55" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y55" s="10">
-        <v>13281</v>
+      <c r="Y55" s="18">
+        <v>13342</v>
       </c>
       <c r="Z55">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="AI55" s="14"/>
       <c r="AJ55" s="14"/>
     </row>
     <row r="56" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y56" s="10">
-        <v>11745</v>
+      <c r="Y56" s="18">
+        <v>11717</v>
       </c>
       <c r="Z56">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="AI56" s="14"/>
       <c r="AJ56" s="14"/>
     </row>
     <row r="57" spans="25:36" x14ac:dyDescent="0.25">
-      <c r="Y57" s="10">
-        <v>10480</v>
+      <c r="Y57" s="18">
+        <v>10438</v>
       </c>
       <c r="Z57">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="AI57" s="14"/>
       <c r="AJ57" s="14"/>
     </row>
     <row r="58" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y58" s="18">
+        <v>10657</v>
+      </c>
+      <c r="Z58">
+        <v>27</v>
+      </c>
       <c r="AI58" s="14"/>
       <c r="AJ58" s="14"/>
     </row>
+    <row r="59" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="AI59" s="14"/>
+      <c r="AJ59" s="14"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Y31:Z57">
-    <sortCondition descending="1" ref="Z31:Z57"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Y32:Z58">
+    <sortCondition ref="Z32:Z58"/>
   </sortState>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7976,7 +8086,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>